<commit_message>
Updated incorrect screws in parts list
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="426">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -82,16 +82,16 @@
     <t>Body, Corner Steering, Differential Pivot, Mechanical Integration, Wheel Assembly</t>
   </si>
   <si>
-    <t>M2.5 x 4mm Screw</t>
+    <t>M2.5 x 6mm Screw</t>
   </si>
   <si>
     <t>B10</t>
   </si>
   <si>
-    <t>91292A015</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/91292A015</t>
+    <t>92095a458</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92095a458</t>
   </si>
   <si>
     <t>Body</t>
@@ -133,10 +133,10 @@
     <t>B13</t>
   </si>
   <si>
-    <t>91255A077</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/91255A077</t>
+    <t>91255A076</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91255A076</t>
   </si>
   <si>
     <t>#6-32 x 3/8 Button Head Screw</t>
@@ -631,6 +631,9 @@
     <t>E5</t>
   </si>
   <si>
+    <t>172:1 gear ratio, with relative encoder</t>
+  </si>
+  <si>
     <t>https://www.pololu.com/product/3268</t>
   </si>
   <si>
@@ -643,6 +646,9 @@
     <t>E6</t>
   </si>
   <si>
+    <t>172:1 gear ratio, NO relative encoder</t>
+  </si>
+  <si>
     <t>https://www.pololu.com/product/3232</t>
   </si>
   <si>
@@ -1219,7 +1225,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Differential Pivot, Body, Rocker-Bogie, Head Assembly, Mechanical Integration, Wheel Assembly</t>
+    <t>Head Assembly, Mechanical Integration, Rocker-Bogie, Differential Pivot, Wheel Assembly, Body</t>
   </si>
   <si>
     <t>Allen Key Set</t>
@@ -1228,7 +1234,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Differential Pivot, Body, Corner Steering, Rocker-Bogie, Head Assembly, Mechanical Integration, Wheel Assembly</t>
+    <t>Head Assembly, Mechanical Integration, Rocker-Bogie, Corner Steering, Differential Pivot, Wheel Assembly, Body</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1237,6 +1243,9 @@
     <t>D7</t>
   </si>
   <si>
+    <t>Wheel Assembly, Differential Pivot</t>
+  </si>
+  <si>
     <t>Hand Drill or Drill Press</t>
   </si>
   <si>
@@ -1255,7 +1264,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Differential Pivot, Corner Steering, Rocker-Bogie, Head Assembly, Wheel Assembly</t>
+    <t>Head Assembly, Rocker-Bogie, Corner Steering, Differential Pivot, Wheel Assembly</t>
   </si>
   <si>
     <t>Vice Clamp or C Clamps</t>
@@ -1264,7 +1273,7 @@
     <t>D5</t>
   </si>
   <si>
-    <t>Differential Pivot, Corner Steering, Wheel Assembly</t>
+    <t>Corner Steering, Wheel Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Vice or V-Clamp</t>
@@ -1785,10 +1794,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>5.61</v>
+        <v>7.07</v>
       </c>
       <c r="J6" s="1">
-        <v>5.61</v>
+        <v>7.07</v>
       </c>
       <c r="K6" t="s">
         <v>25</v>
@@ -1890,10 +1899,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="1">
-        <v>3.78</v>
+        <v>3.76</v>
       </c>
       <c r="J9" s="1">
-        <v>3.78</v>
+        <v>3.76</v>
       </c>
       <c r="K9" t="s">
         <v>25</v>
@@ -3197,11 +3206,14 @@
       <c r="B48" t="s">
         <v>203</v>
       </c>
+      <c r="C48" t="s">
+        <v>204</v>
+      </c>
       <c r="D48" t="s">
         <v>128</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -3219,21 +3231,24 @@
         <v>209.7</v>
       </c>
       <c r="K48" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B49" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="C49" t="s">
+        <v>209</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -3256,19 +3271,19 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D50" t="s">
         <v>88</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -3291,16 +3306,16 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D51" t="s">
         <v>94</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -3318,24 +3333,24 @@
         <v>24.95</v>
       </c>
       <c r="K51" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C52" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D52" t="s">
         <v>133</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -3358,19 +3373,19 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C53">
         <v>585440</v>
       </c>
       <c r="D53" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -3388,24 +3403,24 @@
         <v>17.94</v>
       </c>
       <c r="K53" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B54" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C54">
         <v>535110</v>
       </c>
       <c r="D54" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -3428,19 +3443,19 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B55" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C55">
         <v>535118</v>
       </c>
       <c r="D55" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -3458,24 +3473,24 @@
         <v>41.94</v>
       </c>
       <c r="K55" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B56" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C56">
         <v>545588</v>
       </c>
       <c r="D56" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -3493,24 +3508,24 @@
         <v>23.96</v>
       </c>
       <c r="K56" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B57" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C57">
         <v>545600</v>
       </c>
       <c r="D57" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -3528,24 +3543,24 @@
         <v>17.97</v>
       </c>
       <c r="K57" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B58" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C58">
         <v>545608</v>
       </c>
       <c r="D58" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -3563,24 +3578,24 @@
         <v>35.94</v>
       </c>
       <c r="K58" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C59">
         <v>634066</v>
       </c>
       <c r="D59" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -3603,19 +3618,19 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B60" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C60" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -3638,19 +3653,19 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B61" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C61">
         <v>585470</v>
       </c>
       <c r="D61" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F61">
         <v>2</v>
@@ -3673,19 +3688,19 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B62" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C62">
         <v>635254</v>
       </c>
       <c r="D62" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -3708,19 +3723,19 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B63" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C63">
         <v>635252</v>
       </c>
       <c r="D63" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -3738,24 +3753,24 @@
         <v>1.49</v>
       </c>
       <c r="K63" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B64" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C64">
         <v>585442</v>
       </c>
       <c r="D64" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -3773,24 +3788,24 @@
         <v>71.81999999999999</v>
       </c>
       <c r="K64" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B65" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C65">
         <v>585546</v>
       </c>
       <c r="D65" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -3813,19 +3828,19 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B66" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C66">
         <v>585404</v>
       </c>
       <c r="D66" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F66">
         <v>2</v>
@@ -3848,19 +3863,19 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B67" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C67" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D67" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -3878,24 +3893,24 @@
         <v>24.86</v>
       </c>
       <c r="K67" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B68" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C68">
         <v>625049</v>
       </c>
       <c r="D68" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -3918,19 +3933,19 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B69" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C69">
         <v>545512</v>
       </c>
       <c r="D69" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -3953,19 +3968,19 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B70" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C70">
         <v>545680</v>
       </c>
       <c r="D70" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -3983,24 +3998,24 @@
         <v>35.94</v>
       </c>
       <c r="K70" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B71" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C71" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -4018,24 +4033,24 @@
         <v>14.76</v>
       </c>
       <c r="K71" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B72" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C72">
         <v>615362</v>
       </c>
       <c r="D72" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -4058,16 +4073,16 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B73" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D73" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -4087,19 +4102,19 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B74" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C74" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D74" t="s">
         <v>18</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -4117,24 +4132,24 @@
         <v>4.92</v>
       </c>
       <c r="K74" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B75" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C75">
         <v>585443</v>
       </c>
       <c r="D75" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -4157,16 +4172,16 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B76" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D76" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F76">
         <v>2</v>
@@ -4184,21 +4199,21 @@
         <v>75.81</v>
       </c>
       <c r="K76" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B77" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D77" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -4221,19 +4236,19 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B78" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C78" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D78" t="s">
         <v>82</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F78">
         <v>2</v>
@@ -4256,16 +4271,16 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B79" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D79" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -4285,16 +4300,16 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B80" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -4312,24 +4327,24 @@
         <v>6.49</v>
       </c>
       <c r="K80" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B81" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C81">
         <v>585006</v>
       </c>
       <c r="D81" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -4352,16 +4367,16 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B82" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D82" t="s">
         <v>82</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -4379,24 +4394,24 @@
         <v>5.42</v>
       </c>
       <c r="K82" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B83" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C83">
         <v>585004</v>
       </c>
       <c r="D83" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -4419,16 +4434,16 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B84" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D84" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -4448,19 +4463,19 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B85" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C85">
         <v>585444</v>
       </c>
       <c r="D85" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -4478,24 +4493,24 @@
         <v>19.96</v>
       </c>
       <c r="K85" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B86" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C86">
         <v>585450</v>
       </c>
       <c r="D86" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -4518,19 +4533,19 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B87" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C87">
         <v>545532</v>
       </c>
       <c r="D87" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F87">
         <v>2</v>
@@ -4548,24 +4563,24 @@
         <v>59.85</v>
       </c>
       <c r="K87" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B88" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C88">
         <v>585592</v>
       </c>
       <c r="D88" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -4588,19 +4603,19 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B89" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C89">
         <v>585468</v>
       </c>
       <c r="D89" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -4623,19 +4638,19 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B90" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C90">
         <v>555104</v>
       </c>
       <c r="D90" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -4658,19 +4673,19 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B91" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C91" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -4688,24 +4703,24 @@
         <v>13.8</v>
       </c>
       <c r="K91" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B92" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C92">
         <v>633126</v>
       </c>
       <c r="D92" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F92">
         <v>4</v>
@@ -4723,24 +4738,24 @@
         <v>8.949999999999999</v>
       </c>
       <c r="K92" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B93" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C93" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D93" t="s">
         <v>18</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -4763,19 +4778,19 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B94" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C94" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D94" t="s">
         <v>18</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -4798,19 +4813,19 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B95" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C95" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -4833,19 +4848,19 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B96" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C96" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D96" t="s">
         <v>18</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -4868,19 +4883,19 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B97" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C97" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D97" t="s">
         <v>18</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -4903,19 +4918,19 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B98" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C98" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F98">
         <v>100</v>
@@ -4933,24 +4948,24 @@
         <v>1.17</v>
       </c>
       <c r="K98" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B99" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C99" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D99" t="s">
         <v>18</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="F99">
         <v>100</v>
@@ -4973,19 +4988,19 @@
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B100" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C100" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="F100">
         <v>5</v>
@@ -5003,18 +5018,18 @@
         <v>7.41</v>
       </c>
       <c r="K100" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D101" t="s">
         <v>82</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -5034,13 +5049,13 @@
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D102" t="s">
         <v>82</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -5060,13 +5075,13 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D103" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -5086,13 +5101,13 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" t="s">
+        <v>398</v>
+      </c>
+      <c r="D104" t="s">
         <v>396</v>
       </c>
-      <c r="D104" t="s">
-        <v>394</v>
-      </c>
       <c r="E104" s="5" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -5112,13 +5127,13 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
+        <v>399</v>
+      </c>
+      <c r="D105" t="s">
+        <v>396</v>
+      </c>
+      <c r="E105" s="5" t="s">
         <v>397</v>
-      </c>
-      <c r="D105" t="s">
-        <v>394</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>395</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -5138,122 +5153,122 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B106" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G106">
         <v>1</v>
       </c>
       <c r="K106" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B107" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="G107">
         <v>1</v>
       </c>
       <c r="K107" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B108" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="G108">
         <v>1</v>
       </c>
       <c r="K108" t="s">
-        <v>68</v>
+        <v>408</v>
       </c>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B109" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="G109">
         <v>1</v>
       </c>
       <c r="K109" t="s">
-        <v>68</v>
+        <v>408</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
+        <v>411</v>
+      </c>
+      <c r="B110" t="s">
+        <v>412</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="K110" t="s">
         <v>408</v>
-      </c>
-      <c r="B110" t="s">
-        <v>409</v>
-      </c>
-      <c r="G110">
-        <v>1</v>
-      </c>
-      <c r="K110" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B111" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="G111">
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B112" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="G112">
         <v>1</v>
       </c>
       <c r="K112" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B113" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G113">
         <v>1</v>
       </c>
       <c r="K113" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B114" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="G114">
         <v>1</v>
@@ -5264,10 +5279,10 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B115" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G115">
         <v>1</v>

</xml_diff>

<commit_message>
updating corner steering to use the new shaft clamp, motor, motor mount, etc
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="428">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -1015,6 +1015,15 @@
     <t>S37B</t>
   </si>
   <si>
+    <t>0.25" to 6mm Clamping Shaft Coupler</t>
+  </si>
+  <si>
+    <t>S38</t>
+  </si>
+  <si>
+    <t>https://www.servocity.com/heavy-duty-clamping-shaft-couplers</t>
+  </si>
+  <si>
     <t>4.5” Channel</t>
   </si>
   <si>
@@ -1225,7 +1234,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Differential Pivot, Head Assembly, Wheel Assembly, Corner Steering, Body, Mechanical Integration</t>
+    <t>Corner Steering, Differential Pivot, Mechanical Integration, Rocker-Bogie, Wheel Assembly, Body, Head Assembly</t>
   </si>
   <si>
     <t>5/16 Wrench</t>
@@ -1234,7 +1243,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Differential Pivot, Head Assembly, Wheel Assembly, Body, Mechanical Integration</t>
+    <t>Differential Pivot, Mechanical Integration, Rocker-Bogie, Wheel Assembly, Body, Head Assembly</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1264,22 +1273,22 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Differential Pivot, Head Assembly, Wheel Assembly, Corner Steering</t>
-  </si>
-  <si>
-    <t>Vice Clamp or C Clamps</t>
+    <t>Wheel Assembly, Head Assembly, Rocker-Bogie, Differential Pivot</t>
+  </si>
+  <si>
+    <t>Vice clamp or C Clamps</t>
   </si>
   <si>
     <t>D5</t>
   </si>
   <si>
-    <t>Wheel Assembly, Corner Steering, Differential Pivot</t>
-  </si>
-  <si>
     <t>Vice or V-Clamp</t>
   </si>
   <si>
     <t>D8</t>
+  </si>
+  <si>
+    <t>Head Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Digital Multimeter</t>
@@ -1654,7 +1663,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3913,19 +3922,16 @@
         <v>1</v>
       </c>
       <c r="G68">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H68">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I68" s="1">
         <v>4.99</v>
       </c>
       <c r="J68" s="1">
-        <v>19.96</v>
-      </c>
-      <c r="K68" t="s">
-        <v>59</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -4466,7 +4472,7 @@
         <v>333</v>
       </c>
       <c r="C85">
-        <v>585444</v>
+        <v>625100</v>
       </c>
       <c r="D85" t="s">
         <v>225</v>
@@ -4484,13 +4490,13 @@
         <v>4</v>
       </c>
       <c r="I85" s="1">
-        <v>4.99</v>
+        <v>7.99</v>
       </c>
       <c r="J85" s="1">
-        <v>19.96</v>
+        <v>31.96</v>
       </c>
       <c r="K85" t="s">
-        <v>206</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -4501,7 +4507,7 @@
         <v>336</v>
       </c>
       <c r="C86">
-        <v>585450</v>
+        <v>585444</v>
       </c>
       <c r="D86" t="s">
         <v>225</v>
@@ -4513,19 +4519,19 @@
         <v>1</v>
       </c>
       <c r="G86">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H86">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I86" s="1">
-        <v>7.99</v>
+        <v>4.99</v>
       </c>
       <c r="J86" s="1">
-        <v>15.98</v>
+        <v>19.96</v>
       </c>
       <c r="K86" t="s">
-        <v>54</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4536,7 +4542,7 @@
         <v>339</v>
       </c>
       <c r="C87">
-        <v>545532</v>
+        <v>585450</v>
       </c>
       <c r="D87" t="s">
         <v>225</v>
@@ -4545,57 +4551,57 @@
         <v>340</v>
       </c>
       <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
         <v>2</v>
       </c>
-      <c r="G87">
-        <v>30</v>
-      </c>
       <c r="H87">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I87" s="1">
-        <v>3.99</v>
+        <v>7.99</v>
       </c>
       <c r="J87" s="1">
-        <v>59.85</v>
+        <v>15.98</v>
       </c>
       <c r="K87" t="s">
-        <v>341</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
+        <v>341</v>
+      </c>
+      <c r="B88" t="s">
         <v>342</v>
       </c>
-      <c r="B88" t="s">
-        <v>343</v>
-      </c>
       <c r="C88">
-        <v>585592</v>
+        <v>545532</v>
       </c>
       <c r="D88" t="s">
         <v>225</v>
       </c>
       <c r="E88" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="F88">
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>30</v>
+      </c>
+      <c r="H88">
+        <v>15</v>
+      </c>
+      <c r="I88" s="1">
+        <v>3.99</v>
+      </c>
+      <c r="J88" s="1">
+        <v>59.85</v>
+      </c>
+      <c r="K88" t="s">
         <v>344</v>
-      </c>
-      <c r="F88">
-        <v>1</v>
-      </c>
-      <c r="G88">
-        <v>8</v>
-      </c>
-      <c r="H88">
-        <v>8</v>
-      </c>
-      <c r="I88" s="1">
-        <v>2.79</v>
-      </c>
-      <c r="J88" s="1">
-        <v>22.32</v>
-      </c>
-      <c r="K88" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4606,7 +4612,7 @@
         <v>346</v>
       </c>
       <c r="C89">
-        <v>585468</v>
+        <v>585592</v>
       </c>
       <c r="D89" t="s">
         <v>225</v>
@@ -4618,19 +4624,19 @@
         <v>1</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I89" s="1">
-        <v>1.29</v>
+        <v>2.79</v>
       </c>
       <c r="J89" s="1">
-        <v>1.29</v>
+        <v>22.32</v>
       </c>
       <c r="K89" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4641,7 +4647,7 @@
         <v>349</v>
       </c>
       <c r="C90">
-        <v>555104</v>
+        <v>585468</v>
       </c>
       <c r="D90" t="s">
         <v>225</v>
@@ -4653,19 +4659,19 @@
         <v>1</v>
       </c>
       <c r="G90">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H90">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I90" s="1">
-        <v>3.99</v>
+        <v>1.29</v>
       </c>
       <c r="J90" s="1">
-        <v>15.96</v>
+        <v>1.29</v>
       </c>
       <c r="K90" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4675,134 +4681,134 @@
       <c r="B91" t="s">
         <v>352</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91">
+        <v>555104</v>
+      </c>
+      <c r="D91" t="s">
+        <v>225</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="D91" t="s">
-        <v>18</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>354</v>
-      </c>
       <c r="F91">
         <v>1</v>
       </c>
       <c r="G91">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="H91">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="I91" s="1">
-        <v>0.23</v>
+        <v>3.99</v>
       </c>
       <c r="J91" s="1">
-        <v>13.8</v>
+        <v>15.96</v>
       </c>
       <c r="K91" t="s">
-        <v>355</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
+        <v>354</v>
+      </c>
+      <c r="B92" t="s">
+        <v>355</v>
+      </c>
+      <c r="C92" t="s">
         <v>356</v>
       </c>
-      <c r="B92" t="s">
+      <c r="D92" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="C92">
-        <v>633126</v>
-      </c>
-      <c r="D92" t="s">
-        <v>225</v>
-      </c>
-      <c r="E92" s="5" t="s">
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>60</v>
+      </c>
+      <c r="H92">
+        <v>60</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J92" s="1">
+        <v>13.8</v>
+      </c>
+      <c r="K92" t="s">
         <v>358</v>
-      </c>
-      <c r="F92">
-        <v>4</v>
-      </c>
-      <c r="G92">
-        <v>20</v>
-      </c>
-      <c r="H92">
-        <v>5</v>
-      </c>
-      <c r="I92" s="1">
-        <v>1.79</v>
-      </c>
-      <c r="J92" s="1">
-        <v>8.949999999999999</v>
-      </c>
-      <c r="K92" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
+        <v>359</v>
+      </c>
+      <c r="B93" t="s">
         <v>360</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93">
+        <v>633126</v>
+      </c>
+      <c r="D93" t="s">
+        <v>225</v>
+      </c>
+      <c r="E93" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="C93" t="s">
+      <c r="F93">
+        <v>4</v>
+      </c>
+      <c r="G93">
+        <v>20</v>
+      </c>
+      <c r="H93">
+        <v>5</v>
+      </c>
+      <c r="I93" s="1">
+        <v>1.79</v>
+      </c>
+      <c r="J93" s="1">
+        <v>8.949999999999999</v>
+      </c>
+      <c r="K93" t="s">
         <v>362</v>
-      </c>
-      <c r="D93" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93">
-        <v>8</v>
-      </c>
-      <c r="H93">
-        <v>8</v>
-      </c>
-      <c r="I93" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="J93" s="1">
-        <v>1.84</v>
-      </c>
-      <c r="K93" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
+        <v>363</v>
+      </c>
+      <c r="B94" t="s">
         <v>364</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>365</v>
-      </c>
-      <c r="C94" t="s">
-        <v>366</v>
       </c>
       <c r="D94" t="s">
         <v>18</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F94">
         <v>1</v>
       </c>
       <c r="G94">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H94">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I94" s="1">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="J94" s="1">
-        <v>3.24</v>
+        <v>1.84</v>
       </c>
       <c r="K94" t="s">
         <v>25</v>
@@ -4810,34 +4816,34 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
+        <v>367</v>
+      </c>
+      <c r="B95" t="s">
         <v>368</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>369</v>
-      </c>
-      <c r="C95" t="s">
-        <v>370</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F95">
         <v>1</v>
       </c>
       <c r="G95">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H95">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I95" s="1">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="J95" s="1">
-        <v>2.96</v>
+        <v>3.24</v>
       </c>
       <c r="K95" t="s">
         <v>25</v>
@@ -4857,22 +4863,22 @@
         <v>18</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F96">
         <v>1</v>
       </c>
       <c r="G96">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H96">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I96" s="1">
-        <v>0.48</v>
+        <v>0.37</v>
       </c>
       <c r="J96" s="1">
-        <v>1.92</v>
+        <v>2.96</v>
       </c>
       <c r="K96" t="s">
         <v>25</v>
@@ -4880,31 +4886,31 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
+        <v>374</v>
+      </c>
+      <c r="B97" t="s">
         <v>375</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>376</v>
-      </c>
-      <c r="C97" t="s">
-        <v>377</v>
       </c>
       <c r="D97" t="s">
         <v>18</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F97">
         <v>1</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I97" s="1">
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="J97" s="1">
         <v>1.92</v>
@@ -4915,144 +4921,153 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
+        <v>378</v>
+      </c>
+      <c r="B98" t="s">
         <v>379</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>380</v>
-      </c>
-      <c r="C98" t="s">
-        <v>381</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F98">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G98">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I98" s="1">
-        <v>1.17</v>
+        <v>0.96</v>
       </c>
       <c r="J98" s="1">
-        <v>1.17</v>
+        <v>1.92</v>
       </c>
       <c r="K98" t="s">
-        <v>234</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
+        <v>382</v>
+      </c>
+      <c r="B99" t="s">
         <v>383</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>384</v>
-      </c>
-      <c r="C99" t="s">
-        <v>385</v>
       </c>
       <c r="D99" t="s">
         <v>18</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F99">
         <v>100</v>
       </c>
       <c r="G99">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H99">
         <v>1</v>
       </c>
       <c r="I99" s="1">
-        <v>1.4</v>
+        <v>1.17</v>
       </c>
       <c r="J99" s="1">
-        <v>1.4</v>
+        <v>1.17</v>
       </c>
       <c r="K99" t="s">
-        <v>78</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
+        <v>386</v>
+      </c>
+      <c r="B100" t="s">
         <v>387</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>388</v>
-      </c>
-      <c r="C100" t="s">
-        <v>389</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F100">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G100">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H100">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I100" s="1">
-        <v>2.47</v>
+        <v>1.4</v>
       </c>
       <c r="J100" s="1">
-        <v>7.41</v>
+        <v>1.4</v>
       </c>
       <c r="K100" t="s">
-        <v>276</v>
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
+        <v>390</v>
+      </c>
+      <c r="B101" t="s">
         <v>391</v>
       </c>
+      <c r="C101" t="s">
+        <v>392</v>
+      </c>
       <c r="D101" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G101">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I101" s="1">
-        <v>12.99</v>
+        <v>2.47</v>
       </c>
       <c r="J101" s="1">
-        <v>12.99</v>
+        <v>7.41</v>
+      </c>
+      <c r="K101" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D102" t="s">
         <v>82</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -5064,18 +5079,18 @@
         <v>1</v>
       </c>
       <c r="I102" s="1">
-        <v>25.99</v>
+        <v>12.99</v>
       </c>
       <c r="J102" s="1">
-        <v>25.99</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D103" t="s">
-        <v>396</v>
+        <v>82</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>397</v>
@@ -5090,10 +5105,10 @@
         <v>1</v>
       </c>
       <c r="I103" s="1">
-        <v>20.2</v>
+        <v>25.99</v>
       </c>
       <c r="J103" s="1">
-        <v>20.2</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -5101,10 +5116,10 @@
         <v>398</v>
       </c>
       <c r="D104" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -5116,21 +5131,21 @@
         <v>1</v>
       </c>
       <c r="I104" s="1">
-        <v>19.65</v>
+        <v>20.2</v>
       </c>
       <c r="J104" s="1">
-        <v>19.65</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
+        <v>401</v>
+      </c>
+      <c r="D105" t="s">
         <v>399</v>
       </c>
-      <c r="D105" t="s">
-        <v>396</v>
-      </c>
       <c r="E105" s="5" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -5142,24 +5157,36 @@
         <v>1</v>
       </c>
       <c r="I105" s="1">
-        <v>43.8</v>
+        <v>19.65</v>
       </c>
       <c r="J105" s="1">
-        <v>43.8</v>
+        <v>19.65</v>
       </c>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" t="s">
+        <v>402</v>
+      </c>
+      <c r="D106" t="s">
+        <v>399</v>
+      </c>
+      <c r="E106" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="B106" t="s">
-        <v>401</v>
+      <c r="F106">
+        <v>1</v>
       </c>
       <c r="G106">
         <v>1</v>
       </c>
-      <c r="K106" t="s">
-        <v>402</v>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="I106" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="J106" s="1">
+        <v>43.8</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -5201,35 +5228,35 @@
         <v>1</v>
       </c>
       <c r="K109" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
+        <v>412</v>
+      </c>
+      <c r="B110" t="s">
+        <v>413</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="K110" t="s">
         <v>411</v>
-      </c>
-      <c r="B110" t="s">
-        <v>412</v>
-      </c>
-      <c r="G110">
-        <v>1</v>
-      </c>
-      <c r="K110" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B111" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G111">
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -5257,7 +5284,7 @@
         <v>1</v>
       </c>
       <c r="K113" t="s">
-        <v>35</v>
+        <v>411</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -5271,20 +5298,34 @@
         <v>1</v>
       </c>
       <c r="K114" t="s">
-        <v>135</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B115" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G115">
         <v>1</v>
       </c>
       <c r="K115" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
+      <c r="A116" t="s">
+        <v>426</v>
+      </c>
+      <c r="B116" t="s">
+        <v>427</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="K116" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5378,8 +5419,8 @@
     <hyperlink ref="E89" r:id="rId85"/>
     <hyperlink ref="E90" r:id="rId86"/>
     <hyperlink ref="E91" r:id="rId87"/>
-    <hyperlink ref="E92" r:id="rId88" location="371=256"/>
-    <hyperlink ref="E93" r:id="rId89"/>
+    <hyperlink ref="E92" r:id="rId88"/>
+    <hyperlink ref="E93" r:id="rId89" location="371=256"/>
     <hyperlink ref="E94" r:id="rId90"/>
     <hyperlink ref="E95" r:id="rId91"/>
     <hyperlink ref="E96" r:id="rId92"/>
@@ -5392,6 +5433,7 @@
     <hyperlink ref="E103" r:id="rId99"/>
     <hyperlink ref="E104" r:id="rId100"/>
     <hyperlink ref="E105" r:id="rId101"/>
+    <hyperlink ref="E106" r:id="rId102"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
final commit of all corner steering changes, updated images, CAD files, readme, and more
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="428">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -646,10 +646,13 @@
     <t>E6</t>
   </si>
   <si>
-    <t>172:1 gear ratio, NO relative encoder</t>
-  </si>
-  <si>
-    <t>https://www.pololu.com/product/3232</t>
+    <t>45 RPM HD Premium Planetary Gear Motor, NO relative encoder</t>
+  </si>
+  <si>
+    <t>ServoCity</t>
+  </si>
+  <si>
+    <t>https://www.servocity.com/45-rpm-hd-premium-planetary-gear-motor</t>
   </si>
   <si>
     <t>Absolute Encoder</t>
@@ -694,9 +697,6 @@
     <t>S1</t>
   </si>
   <si>
-    <t>ServoCity</t>
-  </si>
-  <si>
     <t>https://www.servocity.com/1-50-channel</t>
   </si>
   <si>
@@ -1072,13 +1072,13 @@
     <t>https://www.servocity.com/flat-single-channel-bracket</t>
   </si>
   <si>
-    <t>Motor Mount F</t>
+    <t>Motor Mount</t>
   </si>
   <si>
     <t>S9</t>
   </si>
   <si>
-    <t>https://www.servocity.com/aluminum-motor-mount-f</t>
+    <t>https://www.servocity.com/hd-premium-planetary-gear-motor-mount-face-tapped</t>
   </si>
   <si>
     <t>#6 x 1/4 Spacer</t>
@@ -1105,7 +1105,13 @@
     <t>https://www.servocity.com/6-32-thread-1-4-od-round-aluminum-standoffs#371=256</t>
   </si>
   <si>
-    <t>Corner Steering, Wheel Assembly</t>
+    <t>#6-32 x 1.25” Standoff</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>https://www.servocity.com/6-32-thread-1-4-od-round-aluminum-standoffs</t>
   </si>
   <si>
     <t>#4-40 x 1/4 Threaded Standoff</t>
@@ -1234,7 +1240,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Corner Steering, Differential Pivot, Mechanical Integration, Rocker-Bogie, Wheel Assembly, Body, Head Assembly</t>
+    <t>Corner Steering, Body, Differential Pivot, Head Assembly, Rocker-Bogie, Mechanical Integration, Wheel Assembly</t>
   </si>
   <si>
     <t>5/16 Wrench</t>
@@ -1243,7 +1249,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Differential Pivot, Mechanical Integration, Rocker-Bogie, Wheel Assembly, Body, Head Assembly</t>
+    <t>Body, Differential Pivot, Head Assembly, Rocker-Bogie, Mechanical Integration, Wheel Assembly</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1252,9 +1258,6 @@
     <t>D7</t>
   </si>
   <si>
-    <t>Wheel Assembly, Differential Pivot</t>
-  </si>
-  <si>
     <t>Hand Drill or Drill Press</t>
   </si>
   <si>
@@ -1273,7 +1276,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Wheel Assembly, Head Assembly, Rocker-Bogie, Differential Pivot</t>
+    <t>Differential Pivot, Rocker-Bogie, Wheel Assembly, Head Assembly</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1286,9 +1289,6 @@
   </si>
   <si>
     <t>D8</t>
-  </si>
-  <si>
-    <t>Head Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Digital Multimeter</t>
@@ -1663,7 +1663,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K116"/>
+  <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3251,10 +3251,10 @@
         <v>209</v>
       </c>
       <c r="D49" t="s">
-        <v>128</v>
+        <v>210</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -3266,10 +3266,10 @@
         <v>4</v>
       </c>
       <c r="I49" s="1">
-        <v>19.95</v>
+        <v>39.99</v>
       </c>
       <c r="J49" s="1">
-        <v>79.8</v>
+        <v>159.96</v>
       </c>
       <c r="K49" t="s">
         <v>59</v>
@@ -3277,19 +3277,19 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C50" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D50" t="s">
         <v>88</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -3312,16 +3312,16 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D51" t="s">
         <v>94</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -3339,24 +3339,24 @@
         <v>24.95</v>
       </c>
       <c r="K51" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C52" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D52" t="s">
         <v>133</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -3379,16 +3379,16 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C53">
         <v>585440</v>
       </c>
       <c r="D53" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>226</v>
@@ -3423,7 +3423,7 @@
         <v>535110</v>
       </c>
       <c r="D54" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>230</v>
@@ -3458,7 +3458,7 @@
         <v>535118</v>
       </c>
       <c r="D55" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>233</v>
@@ -3493,7 +3493,7 @@
         <v>545588</v>
       </c>
       <c r="D56" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>237</v>
@@ -3528,7 +3528,7 @@
         <v>545600</v>
       </c>
       <c r="D57" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>240</v>
@@ -3563,7 +3563,7 @@
         <v>545608</v>
       </c>
       <c r="D58" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>244</v>
@@ -3598,7 +3598,7 @@
         <v>634066</v>
       </c>
       <c r="D59" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>247</v>
@@ -3668,7 +3668,7 @@
         <v>585470</v>
       </c>
       <c r="D61" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>254</v>
@@ -3703,7 +3703,7 @@
         <v>635254</v>
       </c>
       <c r="D62" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>257</v>
@@ -3738,7 +3738,7 @@
         <v>635252</v>
       </c>
       <c r="D63" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>260</v>
@@ -3773,7 +3773,7 @@
         <v>585442</v>
       </c>
       <c r="D64" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>264</v>
@@ -3808,7 +3808,7 @@
         <v>585546</v>
       </c>
       <c r="D65" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>268</v>
@@ -3843,7 +3843,7 @@
         <v>585404</v>
       </c>
       <c r="D66" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>271</v>
@@ -3878,7 +3878,7 @@
         <v>274</v>
       </c>
       <c r="D67" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>275</v>
@@ -3913,7 +3913,7 @@
         <v>625049</v>
       </c>
       <c r="D68" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>279</v>
@@ -3945,7 +3945,7 @@
         <v>545512</v>
       </c>
       <c r="D69" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>282</v>
@@ -3980,7 +3980,7 @@
         <v>545680</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>285</v>
@@ -4015,7 +4015,7 @@
         <v>288</v>
       </c>
       <c r="D71" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>289</v>
@@ -4050,7 +4050,7 @@
         <v>615362</v>
       </c>
       <c r="D72" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>292</v>
@@ -4135,7 +4135,7 @@
         <v>4.92</v>
       </c>
       <c r="K74" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4149,7 +4149,7 @@
         <v>585443</v>
       </c>
       <c r="D75" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>303</v>
@@ -4344,7 +4344,7 @@
         <v>585006</v>
       </c>
       <c r="D81" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>323</v>
@@ -4411,7 +4411,7 @@
         <v>585004</v>
       </c>
       <c r="D83" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>329</v>
@@ -4475,7 +4475,7 @@
         <v>625100</v>
       </c>
       <c r="D85" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>334</v>
@@ -4510,7 +4510,7 @@
         <v>585444</v>
       </c>
       <c r="D86" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>337</v>
@@ -4545,7 +4545,7 @@
         <v>585450</v>
       </c>
       <c r="D87" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>340</v>
@@ -4580,7 +4580,7 @@
         <v>545532</v>
       </c>
       <c r="D88" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>343</v>
@@ -4615,7 +4615,7 @@
         <v>585592</v>
       </c>
       <c r="D89" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>347</v>
@@ -4650,7 +4650,7 @@
         <v>585468</v>
       </c>
       <c r="D90" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>350</v>
@@ -4681,11 +4681,8 @@
       <c r="B91" t="s">
         <v>352</v>
       </c>
-      <c r="C91">
-        <v>555104</v>
-      </c>
       <c r="D91" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>353</v>
@@ -4700,10 +4697,10 @@
         <v>4</v>
       </c>
       <c r="I91" s="1">
-        <v>3.99</v>
+        <v>4.99</v>
       </c>
       <c r="J91" s="1">
-        <v>15.96</v>
+        <v>19.96</v>
       </c>
       <c r="K91" t="s">
         <v>59</v>
@@ -4755,7 +4752,7 @@
         <v>633126</v>
       </c>
       <c r="D93" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>361</v>
@@ -4764,86 +4761,86 @@
         <v>4</v>
       </c>
       <c r="G93">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="H93">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I93" s="1">
         <v>1.79</v>
       </c>
       <c r="J93" s="1">
-        <v>8.949999999999999</v>
+        <v>1.79</v>
       </c>
       <c r="K93" t="s">
-        <v>362</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
+        <v>362</v>
+      </c>
+      <c r="B94" t="s">
         <v>363</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94">
+        <v>633134</v>
+      </c>
+      <c r="D94" t="s">
+        <v>210</v>
+      </c>
+      <c r="E94" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="C94" t="s">
-        <v>365</v>
-      </c>
-      <c r="D94" t="s">
-        <v>18</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>366</v>
-      </c>
       <c r="F94">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G94">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H94">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I94" s="1">
-        <v>0.23</v>
+        <v>3.29</v>
       </c>
       <c r="J94" s="1">
-        <v>1.84</v>
+        <v>3.29</v>
       </c>
       <c r="K94" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
+        <v>365</v>
+      </c>
+      <c r="B95" t="s">
+        <v>366</v>
+      </c>
+      <c r="C95" t="s">
         <v>367</v>
-      </c>
-      <c r="B95" t="s">
-        <v>368</v>
-      </c>
-      <c r="C95" t="s">
-        <v>369</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F95">
         <v>1</v>
       </c>
       <c r="G95">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H95">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I95" s="1">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="J95" s="1">
-        <v>3.24</v>
+        <v>1.84</v>
       </c>
       <c r="K95" t="s">
         <v>25</v>
@@ -4851,34 +4848,34 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" t="s">
+        <v>369</v>
+      </c>
+      <c r="B96" t="s">
+        <v>370</v>
+      </c>
+      <c r="C96" t="s">
         <v>371</v>
-      </c>
-      <c r="B96" t="s">
-        <v>372</v>
-      </c>
-      <c r="C96" t="s">
-        <v>373</v>
       </c>
       <c r="D96" t="s">
         <v>18</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F96">
         <v>1</v>
       </c>
       <c r="G96">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H96">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I96" s="1">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="J96" s="1">
-        <v>2.96</v>
+        <v>3.24</v>
       </c>
       <c r="K96" t="s">
         <v>25</v>
@@ -4886,34 +4883,34 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
+        <v>373</v>
+      </c>
+      <c r="B97" t="s">
         <v>374</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>375</v>
-      </c>
-      <c r="C97" t="s">
-        <v>376</v>
       </c>
       <c r="D97" t="s">
         <v>18</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F97">
         <v>1</v>
       </c>
       <c r="G97">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H97">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I97" s="1">
-        <v>0.48</v>
+        <v>0.37</v>
       </c>
       <c r="J97" s="1">
-        <v>1.92</v>
+        <v>2.96</v>
       </c>
       <c r="K97" t="s">
         <v>25</v>
@@ -4921,31 +4918,31 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
+        <v>376</v>
+      </c>
+      <c r="B98" t="s">
+        <v>377</v>
+      </c>
+      <c r="C98" t="s">
         <v>378</v>
-      </c>
-      <c r="B98" t="s">
-        <v>379</v>
-      </c>
-      <c r="C98" t="s">
-        <v>380</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F98">
         <v>1</v>
       </c>
       <c r="G98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I98" s="1">
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="J98" s="1">
         <v>1.92</v>
@@ -4956,133 +4953,142 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
+        <v>380</v>
+      </c>
+      <c r="B99" t="s">
+        <v>381</v>
+      </c>
+      <c r="C99" t="s">
         <v>382</v>
-      </c>
-      <c r="B99" t="s">
-        <v>383</v>
-      </c>
-      <c r="C99" t="s">
-        <v>384</v>
       </c>
       <c r="D99" t="s">
         <v>18</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F99">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G99">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I99" s="1">
-        <v>1.17</v>
+        <v>0.96</v>
       </c>
       <c r="J99" s="1">
-        <v>1.17</v>
+        <v>1.92</v>
       </c>
       <c r="K99" t="s">
-        <v>234</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
+        <v>384</v>
+      </c>
+      <c r="B100" t="s">
+        <v>385</v>
+      </c>
+      <c r="C100" t="s">
         <v>386</v>
-      </c>
-      <c r="B100" t="s">
-        <v>387</v>
-      </c>
-      <c r="C100" t="s">
-        <v>388</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F100">
         <v>100</v>
       </c>
       <c r="G100">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100" s="1">
-        <v>1.4</v>
+        <v>1.17</v>
       </c>
       <c r="J100" s="1">
-        <v>1.4</v>
+        <v>1.17</v>
       </c>
       <c r="K100" t="s">
-        <v>78</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
+        <v>388</v>
+      </c>
+      <c r="B101" t="s">
+        <v>389</v>
+      </c>
+      <c r="C101" t="s">
         <v>390</v>
-      </c>
-      <c r="B101" t="s">
-        <v>391</v>
-      </c>
-      <c r="C101" t="s">
-        <v>392</v>
       </c>
       <c r="D101" t="s">
         <v>18</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F101">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G101">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H101">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I101" s="1">
-        <v>2.47</v>
+        <v>1.4</v>
       </c>
       <c r="J101" s="1">
-        <v>7.41</v>
+        <v>1.4</v>
       </c>
       <c r="K101" t="s">
-        <v>276</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
+        <v>392</v>
+      </c>
+      <c r="B102" t="s">
+        <v>393</v>
+      </c>
+      <c r="C102" t="s">
         <v>394</v>
       </c>
       <c r="D102" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>395</v>
       </c>
       <c r="F102">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I102" s="1">
-        <v>12.99</v>
+        <v>2.47</v>
       </c>
       <c r="J102" s="1">
-        <v>12.99</v>
+        <v>7.41</v>
+      </c>
+      <c r="K102" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -5105,10 +5111,10 @@
         <v>1</v>
       </c>
       <c r="I103" s="1">
-        <v>25.99</v>
+        <v>12.99</v>
       </c>
       <c r="J103" s="1">
-        <v>25.99</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -5116,11 +5122,11 @@
         <v>398</v>
       </c>
       <c r="D104" t="s">
+        <v>82</v>
+      </c>
+      <c r="E104" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="E104" s="5" t="s">
-        <v>400</v>
-      </c>
       <c r="F104">
         <v>1</v>
       </c>
@@ -5131,21 +5137,21 @@
         <v>1</v>
       </c>
       <c r="I104" s="1">
-        <v>20.2</v>
+        <v>25.99</v>
       </c>
       <c r="J104" s="1">
-        <v>20.2</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
+        <v>400</v>
+      </c>
+      <c r="D105" t="s">
         <v>401</v>
       </c>
-      <c r="D105" t="s">
-        <v>399</v>
-      </c>
       <c r="E105" s="5" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -5157,22 +5163,22 @@
         <v>1</v>
       </c>
       <c r="I105" s="1">
-        <v>19.65</v>
+        <v>20.2</v>
       </c>
       <c r="J105" s="1">
-        <v>19.65</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" t="s">
+        <v>403</v>
+      </c>
+      <c r="D106" t="s">
+        <v>401</v>
+      </c>
+      <c r="E106" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="D106" t="s">
-        <v>399</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>400</v>
-      </c>
       <c r="F106">
         <v>1</v>
       </c>
@@ -5183,149 +5189,175 @@
         <v>1</v>
       </c>
       <c r="I106" s="1">
-        <v>43.8</v>
+        <v>19.65</v>
       </c>
       <c r="J106" s="1">
-        <v>43.8</v>
+        <v>19.65</v>
       </c>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" t="s">
-        <v>403</v>
-      </c>
-      <c r="B107" t="s">
         <v>404</v>
       </c>
+      <c r="D107" t="s">
+        <v>401</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
       <c r="G107">
         <v>1</v>
       </c>
-      <c r="K107" t="s">
-        <v>405</v>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="J107" s="1">
+        <v>43.8</v>
       </c>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" t="s">
+        <v>405</v>
+      </c>
+      <c r="B108" t="s">
         <v>406</v>
       </c>
-      <c r="B108" t="s">
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="K108" t="s">
         <v>407</v>
-      </c>
-      <c r="G108">
-        <v>1</v>
-      </c>
-      <c r="K108" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" t="s">
+        <v>408</v>
+      </c>
+      <c r="B109" t="s">
         <v>409</v>
       </c>
-      <c r="B109" t="s">
+      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="K109" t="s">
         <v>410</v>
-      </c>
-      <c r="G109">
-        <v>1</v>
-      </c>
-      <c r="K109" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
+        <v>411</v>
+      </c>
+      <c r="B110" t="s">
         <v>412</v>
       </c>
-      <c r="B110" t="s">
-        <v>413</v>
-      </c>
       <c r="G110">
         <v>1</v>
       </c>
       <c r="K110" t="s">
-        <v>411</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
+        <v>413</v>
+      </c>
+      <c r="B111" t="s">
         <v>414</v>
       </c>
-      <c r="B111" t="s">
-        <v>415</v>
-      </c>
       <c r="G111">
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>411</v>
+        <v>68</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
+        <v>415</v>
+      </c>
+      <c r="B112" t="s">
         <v>416</v>
       </c>
-      <c r="B112" t="s">
-        <v>417</v>
-      </c>
       <c r="G112">
         <v>1</v>
       </c>
       <c r="K112" t="s">
-        <v>418</v>
+        <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
+        <v>417</v>
+      </c>
+      <c r="B113" t="s">
+        <v>418</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="K113" t="s">
         <v>419</v>
-      </c>
-      <c r="B113" t="s">
-        <v>420</v>
-      </c>
-      <c r="G113">
-        <v>1</v>
-      </c>
-      <c r="K113" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
+        <v>420</v>
+      </c>
+      <c r="B114" t="s">
         <v>421</v>
       </c>
-      <c r="B114" t="s">
-        <v>422</v>
-      </c>
       <c r="G114">
         <v>1</v>
       </c>
       <c r="K114" t="s">
-        <v>423</v>
+        <v>68</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B115" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G115">
         <v>1</v>
       </c>
       <c r="K115" t="s">
-        <v>135</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
+        <v>424</v>
+      </c>
+      <c r="B116" t="s">
+        <v>425</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="K116" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
+      <c r="A117" t="s">
         <v>426</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>427</v>
       </c>
-      <c r="G116">
-        <v>1</v>
-      </c>
-      <c r="K116" t="s">
+      <c r="G117">
+        <v>1</v>
+      </c>
+      <c r="K117" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5434,6 +5466,7 @@
     <hyperlink ref="E104" r:id="rId100"/>
     <hyperlink ref="E105" r:id="rId101"/>
     <hyperlink ref="E106" r:id="rId102"/>
+    <hyperlink ref="E107" r:id="rId103"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed standoff quantity inconsistency
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="427">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -850,15 +850,6 @@
     <t>Mechanical Integration, Rocker-Bogie</t>
   </si>
   <si>
-    <t>4mm to .25 Clamping Shaft Coupler</t>
-  </si>
-  <si>
-    <t>S23</t>
-  </si>
-  <si>
-    <t>https://www.servocity.com/clamping-shaft-couplers-6776#348=123</t>
-  </si>
-  <si>
     <t>Bore Clamping Hub for 1" PVC</t>
   </si>
   <si>
@@ -1240,7 +1231,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Corner Steering, Body, Differential Pivot, Head Assembly, Rocker-Bogie, Mechanical Integration, Wheel Assembly</t>
+    <t>Head Assembly, Body, Mechanical Integration, Corner Steering, Rocker-Bogie, Wheel Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>5/16 Wrench</t>
@@ -1249,7 +1240,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Body, Differential Pivot, Head Assembly, Rocker-Bogie, Mechanical Integration, Wheel Assembly</t>
+    <t>Head Assembly, Body, Mechanical Integration, Rocker-Bogie, Wheel Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1258,6 +1249,9 @@
     <t>D7</t>
   </si>
   <si>
+    <t>Wheel Assembly, Differential Pivot</t>
+  </si>
+  <si>
     <t>Hand Drill or Drill Press</t>
   </si>
   <si>
@@ -1276,7 +1270,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Differential Pivot, Rocker-Bogie, Wheel Assembly, Head Assembly</t>
+    <t>Wheel Assembly, Head Assembly, Rocker-Bogie, Differential Pivot</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1289,6 +1283,9 @@
   </si>
   <si>
     <t>D8</t>
+  </si>
+  <si>
+    <t>Head Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Digital Multimeter</t>
@@ -1663,7 +1660,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3910,7 +3907,7 @@
         <v>278</v>
       </c>
       <c r="C68">
-        <v>625049</v>
+        <v>545512</v>
       </c>
       <c r="D68" t="s">
         <v>210</v>
@@ -3922,16 +3919,19 @@
         <v>1</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68" s="1">
-        <v>4.99</v>
+        <v>9.99</v>
       </c>
       <c r="J68" s="1">
-        <v>4.99</v>
+        <v>19.98</v>
+      </c>
+      <c r="K68" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -3942,7 +3942,7 @@
         <v>281</v>
       </c>
       <c r="C69">
-        <v>545512</v>
+        <v>545680</v>
       </c>
       <c r="D69" t="s">
         <v>210</v>
@@ -3954,19 +3954,19 @@
         <v>1</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I69" s="1">
-        <v>9.99</v>
+        <v>5.99</v>
       </c>
       <c r="J69" s="1">
-        <v>19.98</v>
+        <v>35.94</v>
       </c>
       <c r="K69" t="s">
-        <v>73</v>
+        <v>206</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3976,29 +3976,29 @@
       <c r="B70" t="s">
         <v>284</v>
       </c>
-      <c r="C70">
-        <v>545680</v>
+      <c r="C70" t="s">
+        <v>285</v>
       </c>
       <c r="D70" t="s">
         <v>210</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F70">
         <v>1</v>
       </c>
       <c r="G70">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H70">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I70" s="1">
-        <v>5.99</v>
+        <v>3.69</v>
       </c>
       <c r="J70" s="1">
-        <v>35.94</v>
+        <v>14.76</v>
       </c>
       <c r="K70" t="s">
         <v>206</v>
@@ -4006,13 +4006,13 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B71" t="s">
-        <v>287</v>
-      </c>
-      <c r="C71" t="s">
         <v>288</v>
+      </c>
+      <c r="C71">
+        <v>615362</v>
       </c>
       <c r="D71" t="s">
         <v>210</v>
@@ -4030,13 +4030,13 @@
         <v>4</v>
       </c>
       <c r="I71" s="1">
-        <v>3.69</v>
+        <v>7.99</v>
       </c>
       <c r="J71" s="1">
-        <v>14.76</v>
+        <v>31.96</v>
       </c>
       <c r="K71" t="s">
-        <v>206</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -4046,46 +4046,43 @@
       <c r="B72" t="s">
         <v>291</v>
       </c>
-      <c r="C72">
-        <v>615362</v>
-      </c>
       <c r="D72" t="s">
-        <v>210</v>
+        <v>292</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F72">
         <v>1</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H72">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I72" s="1">
-        <v>7.99</v>
+        <v>15.25</v>
       </c>
       <c r="J72" s="1">
-        <v>31.96</v>
-      </c>
-      <c r="K72" t="s">
-        <v>59</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B73" t="s">
-        <v>294</v>
+        <v>295</v>
+      </c>
+      <c r="C73" t="s">
+        <v>296</v>
       </c>
       <c r="D73" t="s">
-        <v>295</v>
+        <v>18</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -4097,24 +4094,27 @@
         <v>1</v>
       </c>
       <c r="I73" s="1">
-        <v>15.25</v>
+        <v>4.92</v>
       </c>
       <c r="J73" s="1">
-        <v>15.25</v>
+        <v>4.92</v>
+      </c>
+      <c r="K73" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B74" t="s">
-        <v>298</v>
-      </c>
-      <c r="C74" t="s">
         <v>299</v>
       </c>
+      <c r="C74">
+        <v>585443</v>
+      </c>
       <c r="D74" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>300</v>
@@ -4123,19 +4123,19 @@
         <v>1</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I74" s="1">
-        <v>4.92</v>
+        <v>4.49</v>
       </c>
       <c r="J74" s="1">
-        <v>4.92</v>
+        <v>17.96</v>
       </c>
       <c r="K74" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4145,146 +4145,140 @@
       <c r="B75" t="s">
         <v>302</v>
       </c>
-      <c r="C75">
-        <v>585443</v>
-      </c>
       <c r="D75" t="s">
-        <v>210</v>
+        <v>303</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G75">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H75">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I75" s="1">
-        <v>4.49</v>
+        <v>25.27</v>
       </c>
       <c r="J75" s="1">
-        <v>17.96</v>
+        <v>75.81</v>
       </c>
       <c r="K75" t="s">
-        <v>54</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B76" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D76" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H76">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I76" s="1">
-        <v>25.27</v>
+        <v>12.9</v>
       </c>
       <c r="J76" s="1">
-        <v>75.81</v>
+        <v>51.6</v>
       </c>
       <c r="K76" t="s">
-        <v>206</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B77" t="s">
-        <v>309</v>
+        <v>310</v>
+      </c>
+      <c r="C77" t="s">
+        <v>311</v>
       </c>
       <c r="D77" t="s">
-        <v>310</v>
+        <v>82</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H77">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I77" s="1">
-        <v>12.9</v>
+        <v>9.25</v>
       </c>
       <c r="J77" s="1">
-        <v>51.6</v>
+        <v>9.25</v>
       </c>
       <c r="K77" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B78" t="s">
-        <v>313</v>
-      </c>
-      <c r="C78" t="s">
         <v>314</v>
       </c>
       <c r="D78" t="s">
-        <v>82</v>
+        <v>307</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="F78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78" s="1">
-        <v>9.25</v>
+        <v>75.8</v>
       </c>
       <c r="J78" s="1">
-        <v>9.25</v>
-      </c>
-      <c r="K78" t="s">
-        <v>78</v>
+        <v>75.8</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
+        <v>315</v>
+      </c>
+      <c r="B79" t="s">
         <v>316</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="D79" t="s">
-        <v>310</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>311</v>
-      </c>
       <c r="F79">
         <v>1</v>
       </c>
@@ -4295,10 +4289,13 @@
         <v>1</v>
       </c>
       <c r="I79" s="1">
-        <v>75.8</v>
+        <v>6.49</v>
       </c>
       <c r="J79" s="1">
-        <v>75.8</v>
+        <v>6.49</v>
+      </c>
+      <c r="K79" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -4308,8 +4305,11 @@
       <c r="B80" t="s">
         <v>319</v>
       </c>
+      <c r="C80">
+        <v>585006</v>
+      </c>
       <c r="D80" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>320</v>
@@ -4318,19 +4318,19 @@
         <v>1</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I80" s="1">
-        <v>6.49</v>
+        <v>16.99</v>
       </c>
       <c r="J80" s="1">
-        <v>6.49</v>
+        <v>33.98</v>
       </c>
       <c r="K80" t="s">
-        <v>206</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -4340,11 +4340,8 @@
       <c r="B81" t="s">
         <v>322</v>
       </c>
-      <c r="C81">
-        <v>585006</v>
-      </c>
       <c r="D81" t="s">
-        <v>210</v>
+        <v>82</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>323</v>
@@ -4353,19 +4350,19 @@
         <v>1</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I81" s="1">
-        <v>16.99</v>
+        <v>5.42</v>
       </c>
       <c r="J81" s="1">
-        <v>33.98</v>
+        <v>5.42</v>
       </c>
       <c r="K81" t="s">
-        <v>25</v>
+        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -4375,8 +4372,11 @@
       <c r="B82" t="s">
         <v>325</v>
       </c>
+      <c r="C82">
+        <v>585004</v>
+      </c>
       <c r="D82" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>326</v>
@@ -4385,19 +4385,19 @@
         <v>1</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I82" s="1">
-        <v>5.42</v>
+        <v>13.99</v>
       </c>
       <c r="J82" s="1">
-        <v>5.42</v>
+        <v>41.97</v>
       </c>
       <c r="K82" t="s">
-        <v>206</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -4407,61 +4407,61 @@
       <c r="B83" t="s">
         <v>328</v>
       </c>
-      <c r="C83">
-        <v>585004</v>
-      </c>
       <c r="D83" t="s">
-        <v>210</v>
+        <v>292</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>329</v>
+        <v>293</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I83" s="1">
-        <v>13.99</v>
+        <v>11.75</v>
       </c>
       <c r="J83" s="1">
-        <v>41.97</v>
-      </c>
-      <c r="K83" t="s">
-        <v>25</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" t="s">
+        <v>329</v>
+      </c>
+      <c r="B84" t="s">
         <v>330</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84">
+        <v>625100</v>
+      </c>
+      <c r="D84" t="s">
+        <v>210</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="D84" t="s">
-        <v>295</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>296</v>
-      </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I84" s="1">
-        <v>11.75</v>
+        <v>7.99</v>
       </c>
       <c r="J84" s="1">
-        <v>11.75</v>
+        <v>31.96</v>
+      </c>
+      <c r="K84" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -4472,7 +4472,7 @@
         <v>333</v>
       </c>
       <c r="C85">
-        <v>625100</v>
+        <v>585444</v>
       </c>
       <c r="D85" t="s">
         <v>210</v>
@@ -4490,13 +4490,13 @@
         <v>4</v>
       </c>
       <c r="I85" s="1">
-        <v>7.99</v>
+        <v>4.99</v>
       </c>
       <c r="J85" s="1">
-        <v>31.96</v>
+        <v>19.96</v>
       </c>
       <c r="K85" t="s">
-        <v>59</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -4507,7 +4507,7 @@
         <v>336</v>
       </c>
       <c r="C86">
-        <v>585444</v>
+        <v>585450</v>
       </c>
       <c r="D86" t="s">
         <v>210</v>
@@ -4519,19 +4519,19 @@
         <v>1</v>
       </c>
       <c r="G86">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H86">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I86" s="1">
-        <v>4.99</v>
+        <v>7.99</v>
       </c>
       <c r="J86" s="1">
-        <v>19.96</v>
+        <v>15.98</v>
       </c>
       <c r="K86" t="s">
-        <v>206</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4542,7 +4542,7 @@
         <v>339</v>
       </c>
       <c r="C87">
-        <v>585450</v>
+        <v>545532</v>
       </c>
       <c r="D87" t="s">
         <v>210</v>
@@ -4551,57 +4551,57 @@
         <v>340</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G87">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="H87">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I87" s="1">
-        <v>7.99</v>
+        <v>3.99</v>
       </c>
       <c r="J87" s="1">
-        <v>15.98</v>
+        <v>59.85</v>
       </c>
       <c r="K87" t="s">
-        <v>54</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B88" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C88">
-        <v>545532</v>
+        <v>585592</v>
       </c>
       <c r="D88" t="s">
         <v>210</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G88">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="H88">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I88" s="1">
-        <v>3.99</v>
+        <v>2.79</v>
       </c>
       <c r="J88" s="1">
-        <v>59.85</v>
+        <v>22.32</v>
       </c>
       <c r="K88" t="s">
-        <v>344</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4612,7 +4612,7 @@
         <v>346</v>
       </c>
       <c r="C89">
-        <v>585592</v>
+        <v>585468</v>
       </c>
       <c r="D89" t="s">
         <v>210</v>
@@ -4624,19 +4624,19 @@
         <v>1</v>
       </c>
       <c r="G89">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H89">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I89" s="1">
-        <v>2.79</v>
+        <v>1.29</v>
       </c>
       <c r="J89" s="1">
-        <v>22.32</v>
+        <v>1.29</v>
       </c>
       <c r="K89" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4646,9 +4646,6 @@
       <c r="B90" t="s">
         <v>349</v>
       </c>
-      <c r="C90">
-        <v>585468</v>
-      </c>
       <c r="D90" t="s">
         <v>210</v>
       </c>
@@ -4659,19 +4656,19 @@
         <v>1</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I90" s="1">
-        <v>1.29</v>
+        <v>4.99</v>
       </c>
       <c r="J90" s="1">
-        <v>1.29</v>
+        <v>19.96</v>
       </c>
       <c r="K90" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4681,64 +4678,67 @@
       <c r="B91" t="s">
         <v>352</v>
       </c>
+      <c r="C91" t="s">
+        <v>353</v>
+      </c>
       <c r="D91" t="s">
-        <v>210</v>
+        <v>18</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F91">
         <v>1</v>
       </c>
       <c r="G91">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="H91">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="I91" s="1">
-        <v>4.99</v>
+        <v>0.23</v>
       </c>
       <c r="J91" s="1">
-        <v>19.96</v>
+        <v>13.8</v>
       </c>
       <c r="K91" t="s">
-        <v>59</v>
+        <v>355</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B92" t="s">
-        <v>355</v>
-      </c>
-      <c r="C92" t="s">
-        <v>356</v>
+        <v>357</v>
+      </c>
+      <c r="C92">
+        <v>633126</v>
       </c>
       <c r="D92" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G92">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="H92">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="I92" s="1">
-        <v>0.23</v>
+        <v>1.79</v>
       </c>
       <c r="J92" s="1">
-        <v>13.8</v>
+        <v>1.79</v>
       </c>
       <c r="K92" t="s">
-        <v>358</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -4749,7 +4749,7 @@
         <v>360</v>
       </c>
       <c r="C93">
-        <v>633126</v>
+        <v>633134</v>
       </c>
       <c r="D93" t="s">
         <v>210</v>
@@ -4761,19 +4761,19 @@
         <v>4</v>
       </c>
       <c r="G93">
+        <v>16</v>
+      </c>
+      <c r="H93">
         <v>4</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
       <c r="I93" s="1">
-        <v>1.79</v>
+        <v>3.29</v>
       </c>
       <c r="J93" s="1">
-        <v>1.79</v>
+        <v>13.16</v>
       </c>
       <c r="K93" t="s">
-        <v>206</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -4783,64 +4783,64 @@
       <c r="B94" t="s">
         <v>363</v>
       </c>
-      <c r="C94">
-        <v>633134</v>
+      <c r="C94" t="s">
+        <v>364</v>
       </c>
       <c r="D94" t="s">
-        <v>210</v>
+        <v>18</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F94">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G94">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I94" s="1">
-        <v>3.29</v>
+        <v>0.23</v>
       </c>
       <c r="J94" s="1">
-        <v>3.29</v>
+        <v>1.84</v>
       </c>
       <c r="K94" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B95" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C95" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F95">
         <v>1</v>
       </c>
       <c r="G95">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H95">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I95" s="1">
-        <v>0.23</v>
+        <v>0.27</v>
       </c>
       <c r="J95" s="1">
-        <v>1.84</v>
+        <v>3.24</v>
       </c>
       <c r="K95" t="s">
         <v>25</v>
@@ -4848,34 +4848,34 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B96" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C96" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D96" t="s">
         <v>18</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F96">
         <v>1</v>
       </c>
       <c r="G96">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H96">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I96" s="1">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
       <c r="J96" s="1">
-        <v>3.24</v>
+        <v>2.96</v>
       </c>
       <c r="K96" t="s">
         <v>25</v>
@@ -4895,22 +4895,22 @@
         <v>18</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="F97">
         <v>1</v>
       </c>
       <c r="G97">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H97">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I97" s="1">
-        <v>0.37</v>
+        <v>0.48</v>
       </c>
       <c r="J97" s="1">
-        <v>2.96</v>
+        <v>1.92</v>
       </c>
       <c r="K97" t="s">
         <v>25</v>
@@ -4918,31 +4918,31 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B98" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C98" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F98">
         <v>1</v>
       </c>
       <c r="G98">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H98">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I98" s="1">
-        <v>0.48</v>
+        <v>0.96</v>
       </c>
       <c r="J98" s="1">
         <v>1.92</v>
@@ -4953,153 +4953,144 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B99" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C99" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D99" t="s">
         <v>18</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G99">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="H99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I99" s="1">
-        <v>0.96</v>
+        <v>1.17</v>
       </c>
       <c r="J99" s="1">
-        <v>1.92</v>
+        <v>1.17</v>
       </c>
       <c r="K99" t="s">
-        <v>25</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B100" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C100" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F100">
         <v>100</v>
       </c>
       <c r="G100">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
       <c r="I100" s="1">
-        <v>1.17</v>
+        <v>1.4</v>
       </c>
       <c r="J100" s="1">
-        <v>1.17</v>
+        <v>1.4</v>
       </c>
       <c r="K100" t="s">
-        <v>234</v>
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B101" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C101" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D101" t="s">
         <v>18</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F101">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G101">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I101" s="1">
-        <v>1.4</v>
+        <v>2.47</v>
       </c>
       <c r="J101" s="1">
-        <v>1.4</v>
+        <v>7.41</v>
       </c>
       <c r="K101" t="s">
-        <v>78</v>
+        <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>392</v>
-      </c>
-      <c r="B102" t="s">
         <v>393</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>82</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="D102" t="s">
-        <v>18</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>395</v>
-      </c>
       <c r="F102">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G102">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H102">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I102" s="1">
-        <v>2.47</v>
+        <v>12.99</v>
       </c>
       <c r="J102" s="1">
-        <v>7.41</v>
-      </c>
-      <c r="K102" t="s">
-        <v>276</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D103" t="s">
         <v>82</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -5111,18 +5102,18 @@
         <v>1</v>
       </c>
       <c r="I103" s="1">
-        <v>12.99</v>
+        <v>25.99</v>
       </c>
       <c r="J103" s="1">
-        <v>12.99</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="104" spans="1:11">
       <c r="A104" t="s">
+        <v>397</v>
+      </c>
+      <c r="D104" t="s">
         <v>398</v>
-      </c>
-      <c r="D104" t="s">
-        <v>82</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>399</v>
@@ -5137,10 +5128,10 @@
         <v>1</v>
       </c>
       <c r="I104" s="1">
-        <v>25.99</v>
+        <v>20.2</v>
       </c>
       <c r="J104" s="1">
-        <v>25.99</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -5148,10 +5139,10 @@
         <v>400</v>
       </c>
       <c r="D105" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -5163,21 +5154,21 @@
         <v>1</v>
       </c>
       <c r="I105" s="1">
-        <v>20.2</v>
+        <v>19.65</v>
       </c>
       <c r="J105" s="1">
-        <v>20.2</v>
+        <v>19.65</v>
       </c>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D106" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -5189,36 +5180,24 @@
         <v>1</v>
       </c>
       <c r="I106" s="1">
-        <v>19.65</v>
+        <v>43.8</v>
       </c>
       <c r="J106" s="1">
-        <v>19.65</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" t="s">
+        <v>402</v>
+      </c>
+      <c r="B107" t="s">
+        <v>403</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="K107" t="s">
         <v>404</v>
-      </c>
-      <c r="D107" t="s">
-        <v>401</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="F107">
-        <v>1</v>
-      </c>
-      <c r="G107">
-        <v>1</v>
-      </c>
-      <c r="H107">
-        <v>1</v>
-      </c>
-      <c r="I107" s="1">
-        <v>43.8</v>
-      </c>
-      <c r="J107" s="1">
-        <v>43.8</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -5260,7 +5239,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="s">
-        <v>68</v>
+        <v>410</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -5274,7 +5253,7 @@
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>68</v>
+        <v>410</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -5288,21 +5267,21 @@
         <v>1</v>
       </c>
       <c r="K112" t="s">
-        <v>68</v>
+        <v>417</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B113" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G113">
         <v>1</v>
       </c>
       <c r="K113" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -5316,48 +5295,34 @@
         <v>1</v>
       </c>
       <c r="K114" t="s">
-        <v>68</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B115" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="G115">
         <v>1</v>
       </c>
       <c r="K115" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B116" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G116">
         <v>1</v>
       </c>
       <c r="K116" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11">
-      <c r="A117" t="s">
-        <v>426</v>
-      </c>
-      <c r="B117" t="s">
-        <v>427</v>
-      </c>
-      <c r="G117">
-        <v>1</v>
-      </c>
-      <c r="K117" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5427,10 +5392,10 @@
     <hyperlink ref="E65" r:id="rId61"/>
     <hyperlink ref="E66" r:id="rId62"/>
     <hyperlink ref="E67" r:id="rId63" location="368=229"/>
-    <hyperlink ref="E68" r:id="rId64" location="348=123"/>
+    <hyperlink ref="E68" r:id="rId64"/>
     <hyperlink ref="E69" r:id="rId65"/>
-    <hyperlink ref="E70" r:id="rId66"/>
-    <hyperlink ref="E71" r:id="rId67" location="199=15"/>
+    <hyperlink ref="E70" r:id="rId66" location="199=15"/>
+    <hyperlink ref="E71" r:id="rId67"/>
     <hyperlink ref="E72" r:id="rId68"/>
     <hyperlink ref="E73" r:id="rId69"/>
     <hyperlink ref="E74" r:id="rId70"/>
@@ -5451,8 +5416,8 @@
     <hyperlink ref="E89" r:id="rId85"/>
     <hyperlink ref="E90" r:id="rId86"/>
     <hyperlink ref="E91" r:id="rId87"/>
-    <hyperlink ref="E92" r:id="rId88"/>
-    <hyperlink ref="E93" r:id="rId89" location="371=256"/>
+    <hyperlink ref="E92" r:id="rId88" location="371=256"/>
+    <hyperlink ref="E93" r:id="rId89"/>
     <hyperlink ref="E94" r:id="rId90"/>
     <hyperlink ref="E95" r:id="rId91"/>
     <hyperlink ref="E96" r:id="rId92"/>
@@ -5466,7 +5431,6 @@
     <hyperlink ref="E104" r:id="rId100"/>
     <hyperlink ref="E105" r:id="rId101"/>
     <hyperlink ref="E106" r:id="rId102"/>
-    <hyperlink ref="E107" r:id="rId103"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed model # / link inconsistency for screws in master parts list
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="426">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -160,7 +160,7 @@
     <t>B3</t>
   </si>
   <si>
-    <t>92196A148</t>
+    <t>92949A148</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/92949A148</t>
@@ -175,7 +175,7 @@
     <t>B4</t>
   </si>
   <si>
-    <t>92196A150</t>
+    <t>92949A150</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/92949A150</t>
@@ -190,7 +190,7 @@
     <t>B5</t>
   </si>
   <si>
-    <t>92196A151</t>
+    <t>92949A151</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/92949A151</t>
@@ -205,7 +205,7 @@
     <t>B6</t>
   </si>
   <si>
-    <t>96006A252</t>
+    <t>92949A153</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/92949A153</t>
@@ -1231,7 +1231,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Head Assembly, Body, Mechanical Integration, Corner Steering, Rocker-Bogie, Wheel Assembly, Differential Pivot</t>
+    <t>Rocker-Bogie, Corner Steering, Differential Pivot, Body, Head Assembly, Mechanical Integration, Wheel Assembly</t>
   </si>
   <si>
     <t>5/16 Wrench</t>
@@ -1240,7 +1240,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Head Assembly, Body, Mechanical Integration, Rocker-Bogie, Wheel Assembly, Differential Pivot</t>
+    <t>Rocker-Bogie, Differential Pivot, Body, Head Assembly, Mechanical Integration, Wheel Assembly</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1249,9 +1249,6 @@
     <t>D7</t>
   </si>
   <si>
-    <t>Wheel Assembly, Differential Pivot</t>
-  </si>
-  <si>
     <t>Hand Drill or Drill Press</t>
   </si>
   <si>
@@ -1270,7 +1267,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Wheel Assembly, Head Assembly, Rocker-Bogie, Differential Pivot</t>
+    <t>Rocker-Bogie, Head Assembly, Differential Pivot, Wheel Assembly</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -5225,85 +5222,85 @@
         <v>1</v>
       </c>
       <c r="K109" t="s">
-        <v>410</v>
+        <v>68</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
+        <v>410</v>
+      </c>
+      <c r="B110" t="s">
         <v>411</v>
       </c>
-      <c r="B110" t="s">
-        <v>412</v>
-      </c>
       <c r="G110">
         <v>1</v>
       </c>
       <c r="K110" t="s">
-        <v>410</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
+        <v>412</v>
+      </c>
+      <c r="B111" t="s">
         <v>413</v>
       </c>
-      <c r="B111" t="s">
-        <v>414</v>
-      </c>
       <c r="G111">
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>410</v>
+        <v>68</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
+        <v>414</v>
+      </c>
+      <c r="B112" t="s">
         <v>415</v>
       </c>
-      <c r="B112" t="s">
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="K112" t="s">
         <v>416</v>
-      </c>
-      <c r="G112">
-        <v>1</v>
-      </c>
-      <c r="K112" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
+        <v>417</v>
+      </c>
+      <c r="B113" t="s">
         <v>418</v>
       </c>
-      <c r="B113" t="s">
-        <v>419</v>
-      </c>
       <c r="G113">
         <v>1</v>
       </c>
       <c r="K113" t="s">
-        <v>410</v>
+        <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
+        <v>419</v>
+      </c>
+      <c r="B114" t="s">
         <v>420</v>
       </c>
-      <c r="B114" t="s">
+      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="K114" t="s">
         <v>421</v>
-      </c>
-      <c r="G114">
-        <v>1</v>
-      </c>
-      <c r="K114" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
+        <v>422</v>
+      </c>
+      <c r="B115" t="s">
         <v>423</v>
-      </c>
-      <c r="B115" t="s">
-        <v>424</v>
       </c>
       <c r="G115">
         <v>1</v>
@@ -5314,10 +5311,10 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
+        <v>424</v>
+      </c>
+      <c r="B116" t="s">
         <v>425</v>
-      </c>
-      <c r="B116" t="s">
-        <v>426</v>
       </c>
       <c r="G116">
         <v>1</v>

</xml_diff>

<commit_message>
Uploading fixed version of Drive_motor_mount_v2 for drive motor mounting with servo city motors
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -1677,7 +1677,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
@@ -1750,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>224</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>228</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>235</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>238</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>242</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>245</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>248</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>252</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>258</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>262</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>266</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>269</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>272</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>277</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>280</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>283</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>15.25</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>294</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>298</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>318</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>324</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>329</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>332</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>335</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>338</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>342</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>345</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>348</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>351</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>356</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>359</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>362</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>366</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>370</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>373</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>377</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>381</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>385</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>389</v>
       </c>
@@ -5344,7 +5344,7 @@
   <autoFilter ref="A4:K116">
     <filterColumn colId="3">
       <filters>
-        <filter val="ServoCity"/>
+        <filter val="McMaster"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Updated corner steering D shaft length (closes #114)
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -1231,7 +1231,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Corner Steering, Differential Pivot, Body, Head Assembly, Mechanical Integration, Wheel Assembly</t>
+    <t>Rocker-Bogie, Head Assembly, Body, Wheel Assembly, Differential Pivot, Mechanical Integration, Corner Steering</t>
   </si>
   <si>
     <t>5/16 Wrench</t>
@@ -1240,7 +1240,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Differential Pivot, Body, Head Assembly, Mechanical Integration, Wheel Assembly</t>
+    <t>Rocker-Bogie, Head Assembly, Body, Wheel Assembly, Differential Pivot, Mechanical Integration</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1249,6 +1249,9 @@
     <t>D7</t>
   </si>
   <si>
+    <t>Wheel Assembly, Differential Pivot</t>
+  </si>
+  <si>
     <t>Hand Drill or Drill Press</t>
   </si>
   <si>
@@ -1267,7 +1270,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Head Assembly, Differential Pivot, Wheel Assembly</t>
+    <t>Rocker-Bogie, Wheel Assembly, Differential Pivot, Head Assembly</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1280,9 +1283,6 @@
   </si>
   <si>
     <t>D8</t>
-  </si>
-  <si>
-    <t>Head Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Digital Multimeter</t>
@@ -3589,7 +3589,7 @@
         <v>246</v>
       </c>
       <c r="C59">
-        <v>634066</v>
+        <v>634070</v>
       </c>
       <c r="D59" t="s">
         <v>210</v>
@@ -3607,10 +3607,10 @@
         <v>4</v>
       </c>
       <c r="I59" s="1">
-        <v>1.49</v>
+        <v>1.79</v>
       </c>
       <c r="J59" s="1">
-        <v>5.96</v>
+        <v>7.16</v>
       </c>
       <c r="K59" t="s">
         <v>59</v>
@@ -5222,77 +5222,77 @@
         <v>1</v>
       </c>
       <c r="K109" t="s">
-        <v>68</v>
+        <v>410</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
+        <v>411</v>
+      </c>
+      <c r="B110" t="s">
+        <v>412</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="K110" t="s">
         <v>410</v>
-      </c>
-      <c r="B110" t="s">
-        <v>411</v>
-      </c>
-      <c r="G110">
-        <v>1</v>
-      </c>
-      <c r="K110" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B111" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G111">
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>68</v>
+        <v>410</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B112" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="G112">
         <v>1</v>
       </c>
       <c r="K112" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B113" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G113">
         <v>1</v>
       </c>
       <c r="K113" t="s">
-        <v>68</v>
+        <v>410</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B114" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G114">
         <v>1</v>
       </c>
       <c r="K114" t="s">
-        <v>421</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115" spans="1:11">

</xml_diff>

<commit_message>
Adding 5.2mAH battery mount. Updating the Encoder mount to have notches for clamping screw tightenting
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -1674,11 +1674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2205,7 +2204,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -2345,7 +2344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>41.95</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -2441,7 +2440,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>9.98</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -2505,7 +2504,7 @@
         <v>19.75</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>6.79</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -2738,7 +2737,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>151</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -2840,7 +2839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -2875,7 +2874,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>163</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>167</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>175</v>
       </c>
@@ -3012,7 +3011,7 @@
         <v>6.32</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -3044,7 +3043,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>183</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>187</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>191</v>
       </c>
@@ -3149,7 +3148,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>195</v>
       </c>
@@ -3184,7 +3183,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>199</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>202</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>212</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>220</v>
       </c>
@@ -3388,7 +3387,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>224</v>
       </c>
@@ -3423,7 +3422,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>228</v>
       </c>
@@ -3458,7 +3457,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -3493,7 +3492,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>235</v>
       </c>
@@ -3528,7 +3527,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>238</v>
       </c>
@@ -3563,7 +3562,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>242</v>
       </c>
@@ -3598,7 +3597,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>245</v>
       </c>
@@ -3668,7 +3667,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>252</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -3738,7 +3737,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>258</v>
       </c>
@@ -3773,7 +3772,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>262</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>266</v>
       </c>
@@ -3843,7 +3842,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>269</v>
       </c>
@@ -3878,7 +3877,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>272</v>
       </c>
@@ -3913,7 +3912,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>277</v>
       </c>
@@ -3948,7 +3947,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>280</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>283</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -4053,7 +4052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>290</v>
       </c>
@@ -4117,7 +4116,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>298</v>
       </c>
@@ -4152,7 +4151,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>301</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>305</v>
       </c>
@@ -4216,7 +4215,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>309</v>
       </c>
@@ -4251,7 +4250,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>313</v>
       </c>
@@ -4280,7 +4279,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>315</v>
       </c>
@@ -4312,7 +4311,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>318</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>321</v>
       </c>
@@ -4379,7 +4378,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>324</v>
       </c>
@@ -4414,7 +4413,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>327</v>
       </c>
@@ -4443,7 +4442,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>329</v>
       </c>
@@ -4478,7 +4477,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>332</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>335</v>
       </c>
@@ -4548,7 +4547,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>338</v>
       </c>
@@ -4583,7 +4582,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>342</v>
       </c>
@@ -4618,7 +4617,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>345</v>
       </c>
@@ -4653,7 +4652,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>348</v>
       </c>
@@ -4720,7 +4719,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>356</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>359</v>
       </c>
@@ -5070,7 +5069,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>393</v>
       </c>
@@ -5096,7 +5095,7 @@
         <v>12.99</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>395</v>
       </c>
@@ -5122,7 +5121,7 @@
         <v>25.99</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>397</v>
       </c>
@@ -5148,7 +5147,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>400</v>
       </c>
@@ -5174,7 +5173,7 @@
         <v>19.649999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>401</v>
       </c>
@@ -5200,7 +5199,7 @@
         <v>43.8</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>402</v>
       </c>
@@ -5214,7 +5213,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>405</v>
       </c>
@@ -5228,7 +5227,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>408</v>
       </c>
@@ -5242,7 +5241,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>411</v>
       </c>
@@ -5256,7 +5255,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>413</v>
       </c>
@@ -5270,7 +5269,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>415</v>
       </c>
@@ -5284,7 +5283,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>418</v>
       </c>
@@ -5298,7 +5297,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>420</v>
       </c>
@@ -5312,7 +5311,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>423</v>
       </c>
@@ -5326,7 +5325,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>425</v>
       </c>
@@ -5341,13 +5340,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:K116">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="McMaster"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:K116"/>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1"/>
     <hyperlink ref="E6" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated link for drive motors due to discontinued part
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -634,7 +634,7 @@
     <t>172:1 gear ratio, with relative encoder</t>
   </si>
   <si>
-    <t>https://www.pololu.com/product/3268</t>
+    <t>https://www.pololu.com/product/4888</t>
   </si>
   <si>
     <t>Wheel Assembly</t>
@@ -1231,7 +1231,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Head Assembly, Body, Wheel Assembly, Differential Pivot, Mechanical Integration, Corner Steering</t>
+    <t>Mechanical Integration, Rocker-Bogie, Wheel Assembly, Corner Steering, Body, Differential Pivot, Head Assembly</t>
   </si>
   <si>
     <t>5/16 Wrench</t>
@@ -1240,7 +1240,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Head Assembly, Body, Wheel Assembly, Differential Pivot, Mechanical Integration</t>
+    <t>Mechanical Integration, Rocker-Bogie, Wheel Assembly, Body, Differential Pivot, Head Assembly</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1270,7 +1270,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Wheel Assembly, Differential Pivot, Head Assembly</t>
+    <t>Wheel Assembly, Differential Pivot, Head Assembly, Rocker-Bogie</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>

</xml_diff>

<commit_message>
Changed to shorter screws for wheel assembly.  Closes #125
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -139,759 +139,759 @@
     <t>https://www.mcmaster.com/92949A151</t>
   </si>
   <si>
+    <t>Corner Steering, Wheel Assembly</t>
+  </si>
+  <si>
+    <t>#6-32 x 1.0 Button Head Screw</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>92949A153</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92949A153</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>#6-32 x 1.25 Button Head Screw</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>92949A160</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92949A160</t>
+  </si>
+  <si>
+    <t>Differential Pivot</t>
+  </si>
+  <si>
+    <t>#4-40 x 1/4 Button Head Screw</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>92949A106</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92949a106</t>
+  </si>
+  <si>
+    <t>Head Assembly, PCB Assembly</t>
+  </si>
+  <si>
+    <t>#4-40 x 1.25 Button Head Screw</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>92949A118</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92949A118</t>
+  </si>
+  <si>
+    <t>M2.5 x 6mm Screw</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>92095a458</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92095a458</t>
+  </si>
+  <si>
+    <t>#6-32 Locknuts</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>90631A007</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90631A007</t>
+  </si>
+  <si>
+    <t>Body, Differential Pivot, Rocker-Bogie</t>
+  </si>
+  <si>
+    <t>#4-40 Locknuts</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>90631A005</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90631A005</t>
+  </si>
+  <si>
+    <t>#2-56 x 1/4" Screw</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>91255A076</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91255a077</t>
+  </si>
+  <si>
+    <t>PCB Assembly</t>
+  </si>
+  <si>
+    <t>M3 x 6mm Screw</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>90751A110</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90751a110</t>
+  </si>
+  <si>
+    <t>Head Assembly</t>
+  </si>
+  <si>
+    <t>Red Wire 20AWG</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>CN541R-50-ND</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=CN541R-50-ND</t>
+  </si>
+  <si>
+    <t>Electrical Build, PCB Assembly</t>
+  </si>
+  <si>
+    <t>Black Wire 20AWG</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>CN538B-50-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=CN538B-50-ND</t>
+  </si>
+  <si>
+    <t>White Wire 30AWG</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>1528-1737-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1528-1737-ND</t>
+  </si>
+  <si>
+    <t>Electrical Build</t>
+  </si>
+  <si>
+    <t>Blue Wire 30AWG</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>1528-1734-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1528-1734-ND</t>
+  </si>
+  <si>
+    <t>Yellow Wire 30AWG</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>1528-1735-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1528-1735-ND</t>
+  </si>
+  <si>
+    <t>Green Wire 30AWG</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>1528-1736-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1528-1736-ND</t>
+  </si>
+  <si>
+    <t>Control Board</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/</t>
+  </si>
+  <si>
+    <t>Body, PCB Assembly</t>
+  </si>
+  <si>
+    <t>Arduino Shield</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>Term block 6p side entry</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>ED2744-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/OSTTE060104/ED2744-ND/2351820/?itemSeq=281160152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term block 6P top entry </t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>ED2627-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/OSTTF060161/ED2627-ND/614576/?itemSeq=281160153</t>
+  </si>
+  <si>
+    <t>Connector Header socket 20P 2x10</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>S6106-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/PPPC102LFBN-RC/S6106-ND/807245/?itemSeq=281160175</t>
+  </si>
+  <si>
+    <t>Connector Header socket 5P 5x1</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>S7038-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/PPPC051LFBN-RC/S7038-ND/810177/?itemSeq=281160150</t>
+  </si>
+  <si>
+    <t>Resistors 4.7K 1/4 Watt</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>CF14JT4K70CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=CF14JT4K70CT-ND</t>
+  </si>
+  <si>
+    <t>Resistors 10K 1/4 Watt</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>CF14JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT10K0/CF14JT10K0CT-ND/1830374</t>
+  </si>
+  <si>
+    <t>Resistors 22K 1/4 Watt</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>CF14JT22K0CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT22K0/CF14JT22K0CT-ND/1830383</t>
+  </si>
+  <si>
+    <t>Resistors 10K 1/2 Watt</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>S10KHCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CFM12JT10K0/S10KHCT-ND/2617547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 100nF </t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>399-4454-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/C410C104M5U5TA7200/399-4454-1-ND/818311/?itemSeq=283708856</t>
+  </si>
+  <si>
+    <t>Term block 2P side entry (5.08mm)</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>ED2580-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=ED2580-ND</t>
+  </si>
+  <si>
+    <t>Connector Header pin 40P 2x20</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>S9175-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/SBH11-PBPC-D20-ST-BK/S9175-ND/1990068/?itemSeq=281160147</t>
+  </si>
+  <si>
+    <t>Connector Header pin 6P 6x1</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>455-1708-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/jst-sales-america-inc/B6B-PH-K-S-LF-SN/455-1708-ND/926615</t>
+  </si>
+  <si>
+    <t>0.1"+A72 Pitch Pin Header (40 pins)</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>S1011EC-40-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=S1011EC-40-ND</t>
+  </si>
+  <si>
+    <t>10A Fuse</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>507-1916-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=507-1916-ND</t>
+  </si>
+  <si>
+    <t>Power Diode</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>497-2738-5-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/STPS10L25D/497-2738-5-ND/603763/?itemSeq=281160145</t>
+  </si>
+  <si>
+    <t>Term block 2P side entry</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>277-1721-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/phoenix-contact/1984617/277-1721-ND/950849</t>
+  </si>
+  <si>
+    <t>Connector Header pin 16P 2x8</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>ED10523-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/302-S161/ED10523-ND/2794234/?itemSeq=281160135</t>
+  </si>
+  <si>
+    <t>Roboclaw Motor Driver</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>2x7A</t>
+  </si>
+  <si>
+    <t>Pololu</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/3284</t>
+  </si>
+  <si>
+    <t>Raspberry pi 3 model b</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Raspberry-Model-1-2GHz-64-bit-quad-core/dp/B01CD5VC92/ref=sr_1_3?s=electronics&amp;ie=UTF8&amp;qid=1505769274&amp;sr=1-3&amp;keywords=raspberry+pi+3</t>
+  </si>
+  <si>
+    <t>5V Buck Boost Regulator</t>
+  </si>
+  <si>
+    <t>E22</t>
+  </si>
+  <si>
+    <t>D24V50F5</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/2851</t>
+  </si>
+  <si>
+    <t>12V Regulator</t>
+  </si>
+  <si>
+    <t>E23</t>
+  </si>
+  <si>
+    <t>D24V22F12</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/2855</t>
+  </si>
+  <si>
+    <t>Arduino Uno</t>
+  </si>
+  <si>
+    <t>E24</t>
+  </si>
+  <si>
+    <t>1050-1024-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/A000066/1050-1024-ND/2784006/?itemSeq=283429187</t>
+  </si>
+  <si>
+    <t>Op Amp LM 358P</t>
+  </si>
+  <si>
+    <t>E25</t>
+  </si>
+  <si>
+    <t>296-1395-5-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=296-1395-5-ND</t>
+  </si>
+  <si>
+    <t>Rectangular 6P (1x6) Jumper Cable</t>
+  </si>
+  <si>
+    <t>E26</t>
+  </si>
+  <si>
+    <t>455-3156-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/jst-sales-america-inc/A06KR06KR26E305B/455-3156-ND/6194811</t>
+  </si>
+  <si>
+    <t>USB A to USB Micro Cable (Data)</t>
+  </si>
+  <si>
+    <t>E27</t>
+  </si>
+  <si>
+    <t>380-1430-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stewart-connector/SC-2AMK001F/380-1430-ND/8544576</t>
+  </si>
+  <si>
+    <t>USB A to USB Micro Cable Right Angle</t>
+  </si>
+  <si>
+    <t>E28</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00S8GU03A/ref=crt_ewc_img_dp_2?ie=UTF8&amp;psc=1&amp;smid=A1AMUYYA3CT6HJ</t>
+  </si>
+  <si>
+    <t>Rectangular 40P (2x20) Ribbon Cable</t>
+  </si>
+  <si>
+    <t>E29</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1988</t>
+  </si>
+  <si>
+    <t>Rectangular 16P (2x8) Ribbon Cable</t>
+  </si>
+  <si>
+    <t>E30</t>
+  </si>
+  <si>
+    <t>H3CCH-1606G-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/H3CCH-1606G/H3CCH-1606G-ND/1218559/?itemSeq=281160137</t>
+  </si>
+  <si>
+    <t>4 Position USB Hub</t>
+  </si>
+  <si>
+    <t>E31</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Anker-Ultra-Slim-Portable-Adapter-Notebook/dp/B0192LPK5M/ref=sr_1_7?ie=UTF8&amp;qid=1549577176&amp;sr=8-7&amp;keywords=external+power++usb+hub</t>
+  </si>
+  <si>
+    <t>7 Position USB Hub</t>
+  </si>
+  <si>
+    <t>E32</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Anker-7-Port-Adapter-Charging-iPhone/dp/B014ZQ07NE/ref=sr_1_15?ie=UTF8&amp;qid=1549577308&amp;sr=8-15&amp;keywords=usb+hub</t>
+  </si>
+  <si>
+    <t>DIP IC socket 8P</t>
+  </si>
+  <si>
+    <t>E33</t>
+  </si>
+  <si>
+    <t>AE9986-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/A+08-LC-TT/AE9986-ND/821740/?itemSeq=281160151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB A Connector </t>
+  </si>
+  <si>
+    <t>E34</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/USB-A1HSW6/ED2989-ND/2677750/?itemSeq=283940458</t>
+  </si>
+  <si>
+    <t>Tamiya Connectors</t>
+  </si>
+  <si>
+    <t>E35</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Tamiya-Male-Female-150mm-Venom/dp/B000HKEVH6</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>E36</t>
+  </si>
+  <si>
+    <t>Standard Tamiya Connectors</t>
+  </si>
+  <si>
+    <t>BatterySpace</t>
+  </si>
+  <si>
+    <t>https://www.batteryspace.com/li-ion-battery-14-8v-5-2ah-77wh-8a-rate-for-diving-light---un-38-3-passed.aspx</t>
+  </si>
+  <si>
+    <t>LED Array</t>
+  </si>
+  <si>
+    <t>E37</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/420</t>
+  </si>
+  <si>
+    <t>Battery Volt Meter</t>
+  </si>
+  <si>
+    <t>E38</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DROK-Multimeter-6-5-100V-Backlight-Measuring/dp/B017FSED9I</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>E39</t>
+  </si>
+  <si>
+    <t>432-1282-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/bulgin/C3900BA/1091-1026-ND/2747857</t>
+  </si>
+  <si>
+    <t>3 pin Micro Connectors</t>
+  </si>
+  <si>
+    <t>E40</t>
+  </si>
+  <si>
+    <t>CA-MIC3-W3-NC-1</t>
+  </si>
+  <si>
+    <t>US Digital</t>
+  </si>
+  <si>
+    <t>https://www.usdigital.com/products/cables-connectors/cables/3-pin/CA-MIC3-W3-NC</t>
+  </si>
+  <si>
+    <t>Battery Charger</t>
+  </si>
+  <si>
+    <t>E41</t>
+  </si>
+  <si>
+    <t>https://www.batteryspace.com/smart-charger-3-0a-for-14-8v-li-ion-polymer-battery-pack.aspx</t>
+  </si>
+  <si>
+    <t>Wire Braid</t>
+  </si>
+  <si>
+    <t>E42</t>
+  </si>
+  <si>
+    <t>25Ft 0.1875 Diameter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/16-Wind-Side-Entry-Sleeving/dp/B06XRKMB7N/ref=sr_1_8?keywords=side%2Bentry%2Bwire%2Bwrap&amp;qid=1563912694&amp;s=gateway&amp;sr=8-8&amp;th=1</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>E43</t>
+  </si>
+  <si>
+    <t>8Gb</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SanDisk-Ultra-Micro-Adapter-SDSQUNC-016G-GN6MA/dp/B010Q57SEE</t>
+  </si>
+  <si>
+    <t>Heat Shrink Tubing</t>
+  </si>
+  <si>
+    <t>E44</t>
+  </si>
+  <si>
+    <t>532 pc</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Shrink-Tubing-Black-532pcs-innhom/dp/B075WR9FVL</t>
+  </si>
+  <si>
+    <t>Gear Motor w Relative Enc. (Drive Motor)</t>
+  </si>
+  <si>
+    <t>E45</t>
+  </si>
+  <si>
+    <t>172:1 gear ratio, with relative encoder</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/4888</t>
+  </si>
+  <si>
+    <t>Gear Motor (Corner Motor)</t>
+  </si>
+  <si>
+    <t>E46</t>
+  </si>
+  <si>
+    <t>45 RPM HD Premium Planetary Gear Motor, NO relative encoder</t>
+  </si>
+  <si>
+    <t>ServoCity</t>
+  </si>
+  <si>
+    <t>https://www.servocity.com/45-rpm-hd-premium-planetary-gear-motor</t>
+  </si>
+  <si>
     <t>Corner Steering</t>
   </si>
   <si>
-    <t>#6-32 x 1.0 Button Head Screw</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>92949A153</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/92949A153</t>
-  </si>
-  <si>
-    <t>Body</t>
-  </si>
-  <si>
-    <t>#6-32 x 1.25 Button Head Screw</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>92949A160</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/92949A160</t>
-  </si>
-  <si>
-    <t>Differential Pivot, Wheel Assembly</t>
-  </si>
-  <si>
-    <t>#4-40 x 1/4 Button Head Screw</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>92949A106</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/92949a106</t>
-  </si>
-  <si>
-    <t>Head Assembly, PCB Assembly</t>
-  </si>
-  <si>
-    <t>#4-40 x 1.25 Button Head Screw</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>92949A118</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/92949A118</t>
-  </si>
-  <si>
-    <t>Differential Pivot</t>
-  </si>
-  <si>
-    <t>M2.5 x 6mm Screw</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>92095a458</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/92095a458</t>
-  </si>
-  <si>
-    <t>#6-32 Locknuts</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>90631A007</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/90631A007</t>
-  </si>
-  <si>
-    <t>Body, Differential Pivot, Rocker-Bogie</t>
-  </si>
-  <si>
-    <t>#4-40 Locknuts</t>
-  </si>
-  <si>
-    <t>B12</t>
-  </si>
-  <si>
-    <t>90631A005</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/90631A005</t>
-  </si>
-  <si>
-    <t>#2-56 x 1/4" Screw</t>
-  </si>
-  <si>
-    <t>B13</t>
-  </si>
-  <si>
-    <t>91255A076</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/91255a077</t>
-  </si>
-  <si>
-    <t>PCB Assembly</t>
-  </si>
-  <si>
-    <t>M3 x 6mm Screw</t>
-  </si>
-  <si>
-    <t>B14</t>
-  </si>
-  <si>
-    <t>90751A110</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/90751a110</t>
-  </si>
-  <si>
-    <t>Head Assembly</t>
-  </si>
-  <si>
-    <t>Red Wire 20AWG</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>CN541R-50-ND</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=CN541R-50-ND</t>
-  </si>
-  <si>
-    <t>Electrical Build, PCB Assembly</t>
-  </si>
-  <si>
-    <t>Black Wire 20AWG</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>CN538B-50-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=CN538B-50-ND</t>
-  </si>
-  <si>
-    <t>White Wire 30AWG</t>
-  </si>
-  <si>
-    <t>X3</t>
-  </si>
-  <si>
-    <t>1528-1737-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=1528-1737-ND</t>
-  </si>
-  <si>
-    <t>Electrical Build</t>
-  </si>
-  <si>
-    <t>Blue Wire 30AWG</t>
-  </si>
-  <si>
-    <t>X4</t>
-  </si>
-  <si>
-    <t>1528-1734-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=1528-1734-ND</t>
-  </si>
-  <si>
-    <t>Yellow Wire 30AWG</t>
-  </si>
-  <si>
-    <t>X5</t>
-  </si>
-  <si>
-    <t>1528-1735-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=1528-1735-ND</t>
-  </si>
-  <si>
-    <t>Green Wire 30AWG</t>
-  </si>
-  <si>
-    <t>X6</t>
-  </si>
-  <si>
-    <t>1528-1736-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=1528-1736-ND</t>
-  </si>
-  <si>
-    <t>Control Board</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>JLCPCB</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/</t>
-  </si>
-  <si>
-    <t>Body, PCB Assembly</t>
-  </si>
-  <si>
-    <t>Arduino Shield</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>Term block 6p side entry</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>ED2744-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/OSTTE060104/ED2744-ND/2351820/?itemSeq=281160152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term block 6P top entry </t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>ED2627-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/OSTTF060161/ED2627-ND/614576/?itemSeq=281160153</t>
-  </si>
-  <si>
-    <t>Connector Header socket 20P 2x10</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>S6106-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/PPPC102LFBN-RC/S6106-ND/807245/?itemSeq=281160175</t>
-  </si>
-  <si>
-    <t>Connector Header socket 5P 5x1</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>S7038-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/PPPC051LFBN-RC/S7038-ND/810177/?itemSeq=281160150</t>
-  </si>
-  <si>
-    <t>Resistors 4.7K 1/4 Watt</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>CF14JT4K70CT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=CF14JT4K70CT-ND</t>
-  </si>
-  <si>
-    <t>Resistors 10K 1/4 Watt</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>CF14JT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT10K0/CF14JT10K0CT-ND/1830374</t>
-  </si>
-  <si>
-    <t>Resistors 22K 1/4 Watt</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>CF14JT22K0CT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT22K0/CF14JT22K0CT-ND/1830383</t>
-  </si>
-  <si>
-    <t>Resistors 10K 1/2 Watt</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>S10KHCT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CFM12JT10K0/S10KHCT-ND/2617547</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor 100nF </t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>399-4454-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/C410C104M5U5TA7200/399-4454-1-ND/818311/?itemSeq=283708856</t>
-  </si>
-  <si>
-    <t>Term block 2P side entry (5.08mm)</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>ED2580-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=ED2580-ND</t>
-  </si>
-  <si>
-    <t>Connector Header pin 40P 2x20</t>
-  </si>
-  <si>
-    <t>E13</t>
-  </si>
-  <si>
-    <t>S9175-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/SBH11-PBPC-D20-ST-BK/S9175-ND/1990068/?itemSeq=281160147</t>
-  </si>
-  <si>
-    <t>Connector Header pin 6P 6x1</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>455-1708-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/jst-sales-america-inc/B6B-PH-K-S-LF-SN/455-1708-ND/926615</t>
-  </si>
-  <si>
-    <t>0.1"+A72 Pitch Pin Header (40 pins)</t>
-  </si>
-  <si>
-    <t>E15</t>
-  </si>
-  <si>
-    <t>S1011EC-40-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=S1011EC-40-ND</t>
-  </si>
-  <si>
-    <t>10A Fuse</t>
-  </si>
-  <si>
-    <t>E16</t>
-  </si>
-  <si>
-    <t>507-1916-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=507-1916-ND</t>
-  </si>
-  <si>
-    <t>Power Diode</t>
-  </si>
-  <si>
-    <t>E17</t>
-  </si>
-  <si>
-    <t>497-2738-5-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/STPS10L25D/497-2738-5-ND/603763/?itemSeq=281160145</t>
-  </si>
-  <si>
-    <t>Term block 2P side entry</t>
-  </si>
-  <si>
-    <t>E18</t>
-  </si>
-  <si>
-    <t>277-1721-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/phoenix-contact/1984617/277-1721-ND/950849</t>
-  </si>
-  <si>
-    <t>Connector Header pin 16P 2x8</t>
-  </si>
-  <si>
-    <t>E19</t>
-  </si>
-  <si>
-    <t>ED10523-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/302-S161/ED10523-ND/2794234/?itemSeq=281160135</t>
-  </si>
-  <si>
-    <t>Roboclaw Motor Driver</t>
-  </si>
-  <si>
-    <t>E20</t>
-  </si>
-  <si>
-    <t>2x7A</t>
-  </si>
-  <si>
-    <t>Pololu</t>
-  </si>
-  <si>
-    <t>https://www.pololu.com/product/3284</t>
-  </si>
-  <si>
-    <t>Raspberry pi 3 model b</t>
-  </si>
-  <si>
-    <t>E21</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Raspberry-Model-1-2GHz-64-bit-quad-core/dp/B01CD5VC92/ref=sr_1_3?s=electronics&amp;ie=UTF8&amp;qid=1505769274&amp;sr=1-3&amp;keywords=raspberry+pi+3</t>
-  </si>
-  <si>
-    <t>5V Buck Boost Regulator</t>
-  </si>
-  <si>
-    <t>E22</t>
-  </si>
-  <si>
-    <t>D24V50F5</t>
-  </si>
-  <si>
-    <t>https://www.pololu.com/product/2851</t>
-  </si>
-  <si>
-    <t>12V Regulator</t>
-  </si>
-  <si>
-    <t>E23</t>
-  </si>
-  <si>
-    <t>D24V22F12</t>
-  </si>
-  <si>
-    <t>https://www.pololu.com/product/2855</t>
-  </si>
-  <si>
-    <t>Arduino Uno</t>
-  </si>
-  <si>
-    <t>E24</t>
-  </si>
-  <si>
-    <t>1050-1024-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/A000066/1050-1024-ND/2784006/?itemSeq=283429187</t>
-  </si>
-  <si>
-    <t>Op Amp LM 358P</t>
-  </si>
-  <si>
-    <t>E25</t>
-  </si>
-  <si>
-    <t>296-1395-5-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=296-1395-5-ND</t>
-  </si>
-  <si>
-    <t>Rectangular 6P (1x6) Jumper Cable</t>
-  </si>
-  <si>
-    <t>E26</t>
-  </si>
-  <si>
-    <t>455-3156-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/jst-sales-america-inc/A06KR06KR26E305B/455-3156-ND/6194811</t>
-  </si>
-  <si>
-    <t>USB A to USB Micro Cable (Data)</t>
-  </si>
-  <si>
-    <t>E27</t>
-  </si>
-  <si>
-    <t>380-1430-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stewart-connector/SC-2AMK001F/380-1430-ND/8544576</t>
-  </si>
-  <si>
-    <t>USB A to USB Micro Cable Right Angle</t>
-  </si>
-  <si>
-    <t>E28</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B00S8GU03A/ref=crt_ewc_img_dp_2?ie=UTF8&amp;psc=1&amp;smid=A1AMUYYA3CT6HJ</t>
-  </si>
-  <si>
-    <t>Rectangular 40P (2x20) Ribbon Cable</t>
-  </si>
-  <si>
-    <t>E29</t>
-  </si>
-  <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/1988</t>
-  </si>
-  <si>
-    <t>Rectangular 16P (2x8) Ribbon Cable</t>
-  </si>
-  <si>
-    <t>E30</t>
-  </si>
-  <si>
-    <t>H3CCH-1606G-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/H3CCH-1606G/H3CCH-1606G-ND/1218559/?itemSeq=281160137</t>
-  </si>
-  <si>
-    <t>4 Position USB Hub</t>
-  </si>
-  <si>
-    <t>E31</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Anker-Ultra-Slim-Portable-Adapter-Notebook/dp/B0192LPK5M/ref=sr_1_7?ie=UTF8&amp;qid=1549577176&amp;sr=8-7&amp;keywords=external+power++usb+hub</t>
-  </si>
-  <si>
-    <t>7 Position USB Hub</t>
-  </si>
-  <si>
-    <t>E32</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Anker-7-Port-Adapter-Charging-iPhone/dp/B014ZQ07NE/ref=sr_1_15?ie=UTF8&amp;qid=1549577308&amp;sr=8-15&amp;keywords=usb+hub</t>
-  </si>
-  <si>
-    <t>DIP IC socket 8P</t>
-  </si>
-  <si>
-    <t>E33</t>
-  </si>
-  <si>
-    <t>AE9986-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/A+08-LC-TT/AE9986-ND/821740/?itemSeq=281160151</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB A Connector </t>
-  </si>
-  <si>
-    <t>E34</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/USB-A1HSW6/ED2989-ND/2677750/?itemSeq=283940458</t>
-  </si>
-  <si>
-    <t>Tamiya Connectors</t>
-  </si>
-  <si>
-    <t>E35</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Tamiya-Male-Female-150mm-Venom/dp/B000HKEVH6</t>
-  </si>
-  <si>
-    <t>Battery</t>
-  </si>
-  <si>
-    <t>E36</t>
-  </si>
-  <si>
-    <t>Standard Tamiya Connectors</t>
-  </si>
-  <si>
-    <t>BatterySpace</t>
-  </si>
-  <si>
-    <t>https://www.batteryspace.com/li-ion-battery-14-8v-5-2ah-77wh-8a-rate-for-diving-light---un-38-3-passed.aspx</t>
-  </si>
-  <si>
-    <t>LED Array</t>
-  </si>
-  <si>
-    <t>E37</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/420</t>
-  </si>
-  <si>
-    <t>Battery Volt Meter</t>
-  </si>
-  <si>
-    <t>E38</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/DROK-Multimeter-6-5-100V-Backlight-Measuring/dp/B017FSED9I</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>E39</t>
-  </si>
-  <si>
-    <t>432-1282-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/bulgin/C3900BA/1091-1026-ND/2747857</t>
-  </si>
-  <si>
-    <t>3 pin Micro Connectors</t>
-  </si>
-  <si>
-    <t>E40</t>
-  </si>
-  <si>
-    <t>CA-MIC3-W3-NC-1</t>
-  </si>
-  <si>
-    <t>US Digital</t>
-  </si>
-  <si>
-    <t>https://www.usdigital.com/products/cables-connectors/cables/3-pin/CA-MIC3-W3-NC</t>
-  </si>
-  <si>
-    <t>Battery Charger</t>
-  </si>
-  <si>
-    <t>E41</t>
-  </si>
-  <si>
-    <t>https://www.batteryspace.com/smart-charger-3-0a-for-14-8v-li-ion-polymer-battery-pack.aspx</t>
-  </si>
-  <si>
-    <t>Wire Braid</t>
-  </si>
-  <si>
-    <t>E42</t>
-  </si>
-  <si>
-    <t>25Ft 0.1875 Diameter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/16-Wind-Side-Entry-Sleeving/dp/B06XRKMB7N/ref=sr_1_8?keywords=side%2Bentry%2Bwire%2Bwrap&amp;qid=1563912694&amp;s=gateway&amp;sr=8-8&amp;th=1</t>
-  </si>
-  <si>
-    <t>SD Card</t>
-  </si>
-  <si>
-    <t>E43</t>
-  </si>
-  <si>
-    <t>8Gb</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/SanDisk-Ultra-Micro-Adapter-SDSQUNC-016G-GN6MA/dp/B010Q57SEE</t>
-  </si>
-  <si>
-    <t>Heat Shrink Tubing</t>
-  </si>
-  <si>
-    <t>E44</t>
-  </si>
-  <si>
-    <t>532 pc</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Shrink-Tubing-Black-532pcs-innhom/dp/B075WR9FVL</t>
-  </si>
-  <si>
-    <t>Gear Motor w Relative Enc. (Drive Motor)</t>
-  </si>
-  <si>
-    <t>E45</t>
-  </si>
-  <si>
-    <t>172:1 gear ratio, with relative encoder</t>
-  </si>
-  <si>
-    <t>https://www.pololu.com/product/4888</t>
-  </si>
-  <si>
-    <t>Gear Motor (Corner Motor)</t>
-  </si>
-  <si>
-    <t>E46</t>
-  </si>
-  <si>
-    <t>45 RPM HD Premium Planetary Gear Motor, NO relative encoder</t>
-  </si>
-  <si>
-    <t>ServoCity</t>
-  </si>
-  <si>
-    <t>https://www.servocity.com/45-rpm-hd-premium-planetary-gear-motor</t>
-  </si>
-  <si>
     <t>Absolute Encoder</t>
   </si>
   <si>
@@ -1522,7 +1522,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Body, Corner Steering, Differential Pivot, Mechanical Integration, Wheel Assembly, Rocker-Bogie</t>
+    <t>Rocker-Bogie, Differential Pivot, Corner Steering, Wheel Assembly, Mechanical Integration, Body</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1552,7 +1552,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Head Assembly, Wheel Assembly, Differential Pivot</t>
+    <t>Head Assembly, Wheel Assembly, Rocker-Bogie, Differential Pivot</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1567,7 +1567,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Wheel Assembly, Differential Pivot, Mechanical Integration</t>
+    <t>Rocker-Bogie, Wheel Assembly, Mechanical Integration, Differential Pivot</t>
   </si>
   <si>
     <t>Vice or V-Clamp</t>
@@ -2175,7 +2175,7 @@
         <v>100</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2245,7 +2245,7 @@
         <v>50</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2327,24 +2327,24 @@
         <v>7.7</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>25</v>
@@ -2367,19 +2367,19 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>65</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15">
         <v>100</v>
@@ -2397,24 +2397,24 @@
         <v>2.72</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>71</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -2432,24 +2432,24 @@
         <v>2.79</v>
       </c>
       <c r="K16" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>75</v>
-      </c>
-      <c r="C17" t="s">
-        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17">
         <v>25</v>
@@ -2467,24 +2467,24 @@
         <v>3.78</v>
       </c>
       <c r="K17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
         <v>79</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>80</v>
-      </c>
-      <c r="C18" t="s">
-        <v>81</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -2502,24 +2502,24 @@
         <v>6.33</v>
       </c>
       <c r="K18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>85</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>86</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2537,24 +2537,24 @@
         <v>31.18</v>
       </c>
       <c r="K19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2572,24 +2572,24 @@
         <v>25.12</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
         <v>94</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>95</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="D21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2607,24 +2607,24 @@
         <v>4.95</v>
       </c>
       <c r="K21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
         <v>99</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>100</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2642,24 +2642,24 @@
         <v>4.95</v>
       </c>
       <c r="K22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
         <v>103</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>104</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2677,24 +2677,24 @@
         <v>4.95</v>
       </c>
       <c r="K23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
         <v>107</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>108</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="D24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2712,21 +2712,21 @@
         <v>4.95</v>
       </c>
       <c r="K24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
         <v>111</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -2744,21 +2744,21 @@
         <v>22.1</v>
       </c>
       <c r="K25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
         <v>116</v>
       </c>
-      <c r="B26" t="s">
-        <v>117</v>
-      </c>
       <c r="D26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="F26">
         <v>10</v>
@@ -2781,19 +2781,19 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" t="s">
         <v>118</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>119</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2811,24 +2811,24 @@
         <v>14.88</v>
       </c>
       <c r="K27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>123</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="D28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2846,24 +2846,24 @@
         <v>12.18</v>
       </c>
       <c r="K28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
         <v>126</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>127</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="D29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2881,24 +2881,24 @@
         <v>7.56</v>
       </c>
       <c r="K29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" t="s">
         <v>130</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>131</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="D30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2916,24 +2916,24 @@
         <v>3.92</v>
       </c>
       <c r="K30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
         <v>134</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>135</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="F31">
         <v>10</v>
@@ -2951,24 +2951,24 @@
         <v>0.04</v>
       </c>
       <c r="K31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
         <v>138</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>139</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="D32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -2986,24 +2986,24 @@
         <v>0.04</v>
       </c>
       <c r="K32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" t="s">
         <v>142</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>143</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="D33" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="F33">
         <v>10</v>
@@ -3021,24 +3021,24 @@
         <v>0.04</v>
       </c>
       <c r="K33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" t="s">
         <v>146</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>147</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="D34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="F34">
         <v>10</v>
@@ -3056,24 +3056,24 @@
         <v>0.06</v>
       </c>
       <c r="K34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" t="s">
         <v>150</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>151</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="D35" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3091,24 +3091,24 @@
         <v>5.4</v>
       </c>
       <c r="K35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
         <v>154</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>155</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="D36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3126,24 +3126,24 @@
         <v>3</v>
       </c>
       <c r="K36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
         <v>158</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>159</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -3161,24 +3161,24 @@
         <v>2.19</v>
       </c>
       <c r="K37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" t="s">
         <v>162</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>163</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="D38" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -3196,24 +3196,24 @@
         <v>1.98</v>
       </c>
       <c r="K38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" t="s">
         <v>166</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>167</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="D39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -3231,24 +3231,24 @@
         <v>2.95</v>
       </c>
       <c r="K39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" t="s">
         <v>170</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>171</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="D40" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -3266,24 +3266,24 @@
         <v>1.05</v>
       </c>
       <c r="K40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" t="s">
         <v>174</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>175</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -3301,24 +3301,24 @@
         <v>1.55</v>
       </c>
       <c r="K41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" t="s">
         <v>178</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>179</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="D42" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -3336,24 +3336,24 @@
         <v>1.44</v>
       </c>
       <c r="K42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" t="s">
         <v>182</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>183</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -3371,24 +3371,24 @@
         <v>0.84</v>
       </c>
       <c r="K43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" t="s">
         <v>186</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>187</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>188</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -3406,24 +3406,24 @@
         <v>349.75</v>
       </c>
       <c r="K44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" t="s">
         <v>191</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>192</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>193</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -3441,24 +3441,24 @@
         <v>34.99</v>
       </c>
       <c r="K45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" t="s">
         <v>196</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>197</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="D46" t="s">
-        <v>189</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -3476,24 +3476,24 @@
         <v>14.95</v>
       </c>
       <c r="K46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
+        <v>199</v>
+      </c>
+      <c r="B47" t="s">
         <v>200</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>201</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="D47" t="s">
-        <v>189</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -3511,24 +3511,24 @@
         <v>9.949999999999999</v>
       </c>
       <c r="K47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" t="s">
         <v>204</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>205</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="D48" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -3551,19 +3551,19 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" t="s">
         <v>208</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>209</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="D49" t="s">
-        <v>87</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -3581,24 +3581,24 @@
         <v>1.48</v>
       </c>
       <c r="K49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" t="s">
         <v>212</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>213</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="D50" t="s">
-        <v>87</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -3616,24 +3616,24 @@
         <v>1.55</v>
       </c>
       <c r="K50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51" t="s">
         <v>216</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>217</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="D51" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -3651,21 +3651,21 @@
         <v>12.3</v>
       </c>
       <c r="K51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" t="s">
         <v>220</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
+        <v>193</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="D52" t="s">
-        <v>194</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -3683,24 +3683,24 @@
         <v>7.99</v>
       </c>
       <c r="K52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" t="s">
         <v>223</v>
-      </c>
-      <c r="B53" t="s">
-        <v>224</v>
       </c>
       <c r="C53">
         <v>1988</v>
       </c>
       <c r="D53" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -3718,24 +3718,24 @@
         <v>2.95</v>
       </c>
       <c r="K53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
+        <v>226</v>
+      </c>
+      <c r="B54" t="s">
         <v>227</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>228</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="D54" t="s">
-        <v>87</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -3753,21 +3753,21 @@
         <v>1.4</v>
       </c>
       <c r="K54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" t="s">
         <v>231</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="D55" t="s">
-        <v>194</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -3787,16 +3787,16 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
+        <v>233</v>
+      </c>
+      <c r="B56" t="s">
         <v>234</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
+        <v>193</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="D56" t="s">
-        <v>194</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -3816,19 +3816,19 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
+        <v>236</v>
+      </c>
+      <c r="B57" t="s">
         <v>237</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>238</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="D57" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -3846,21 +3846,21 @@
         <v>0.51</v>
       </c>
       <c r="K57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
+        <v>240</v>
+      </c>
+      <c r="B58" t="s">
         <v>241</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="D58" t="s">
-        <v>87</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -3878,24 +3878,24 @@
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
+        <v>243</v>
+      </c>
+      <c r="B59" t="s">
         <v>244</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>182</v>
+      </c>
+      <c r="D59" t="s">
+        <v>193</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="C59" t="s">
-        <v>183</v>
-      </c>
-      <c r="D59" t="s">
-        <v>194</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -3913,24 +3913,24 @@
         <v>5.57</v>
       </c>
       <c r="K59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" t="s">
         <v>247</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>248</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>249</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -3948,21 +3948,21 @@
         <v>86.95</v>
       </c>
       <c r="K60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" t="s">
         <v>252</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
+        <v>224</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="D61" t="s">
-        <v>225</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -3985,16 +3985,16 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
+        <v>254</v>
+      </c>
+      <c r="B62" t="s">
         <v>255</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
+        <v>193</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="D62" t="s">
-        <v>194</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -4017,19 +4017,19 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
+        <v>257</v>
+      </c>
+      <c r="B63" t="s">
         <v>258</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>259</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="D63" t="s">
-        <v>87</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -4052,19 +4052,19 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
+        <v>261</v>
+      </c>
+      <c r="B64" t="s">
         <v>262</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>263</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>264</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -4082,24 +4082,24 @@
         <v>27.2</v>
       </c>
       <c r="K64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
+        <v>266</v>
+      </c>
+      <c r="B65" t="s">
         <v>267</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>248</v>
+      </c>
+      <c r="D65" t="s">
+        <v>249</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C65" t="s">
-        <v>249</v>
-      </c>
-      <c r="D65" t="s">
-        <v>250</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -4117,24 +4117,24 @@
         <v>41.95</v>
       </c>
       <c r="K65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
+        <v>269</v>
+      </c>
+      <c r="B66" t="s">
         <v>270</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>271</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
+        <v>193</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="D66" t="s">
-        <v>194</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -4152,24 +4152,24 @@
         <v>15</v>
       </c>
       <c r="K66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
+        <v>273</v>
+      </c>
+      <c r="B67" t="s">
         <v>274</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>275</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
+        <v>193</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="D67" t="s">
-        <v>194</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -4189,19 +4189,19 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
+        <v>277</v>
+      </c>
+      <c r="B68" t="s">
         <v>278</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>279</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
+        <v>193</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="D68" t="s">
-        <v>194</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -4219,24 +4219,24 @@
         <v>7.99</v>
       </c>
       <c r="K68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
+        <v>281</v>
+      </c>
+      <c r="B69" t="s">
         <v>282</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>283</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>188</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="D69" t="s">
-        <v>189</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -4259,19 +4259,19 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
+        <v>285</v>
+      </c>
+      <c r="B70" t="s">
         <v>286</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>287</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>288</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -4289,7 +4289,7 @@
         <v>159.96</v>
       </c>
       <c r="K70" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -4303,7 +4303,7 @@
         <v>293</v>
       </c>
       <c r="D71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>294</v>
@@ -4324,7 +4324,7 @@
         <v>222</v>
       </c>
       <c r="K71" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -4335,7 +4335,7 @@
         <v>296</v>
       </c>
       <c r="D72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>297</v>
@@ -4356,7 +4356,7 @@
         <v>6.99</v>
       </c>
       <c r="K72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -4370,7 +4370,7 @@
         <v>585440</v>
       </c>
       <c r="D73" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>300</v>
@@ -4405,7 +4405,7 @@
         <v>535110</v>
       </c>
       <c r="D74" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>304</v>
@@ -4426,7 +4426,7 @@
         <v>47.92</v>
       </c>
       <c r="K74" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4440,7 +4440,7 @@
         <v>535118</v>
       </c>
       <c r="D75" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>307</v>
@@ -4475,7 +4475,7 @@
         <v>545588</v>
       </c>
       <c r="D76" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>311</v>
@@ -4510,7 +4510,7 @@
         <v>545600</v>
       </c>
       <c r="D77" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>314</v>
@@ -4531,7 +4531,7 @@
         <v>23.96</v>
       </c>
       <c r="K77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -4545,7 +4545,7 @@
         <v>545608</v>
       </c>
       <c r="D78" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>317</v>
@@ -4580,7 +4580,7 @@
         <v>634070</v>
       </c>
       <c r="D79" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>320</v>
@@ -4601,7 +4601,7 @@
         <v>7.16</v>
       </c>
       <c r="K79" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -4636,7 +4636,7 @@
         <v>23.16</v>
       </c>
       <c r="K80" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -4650,7 +4650,7 @@
         <v>585470</v>
       </c>
       <c r="D81" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>327</v>
@@ -4685,7 +4685,7 @@
         <v>635254</v>
       </c>
       <c r="D82" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>330</v>
@@ -4720,7 +4720,7 @@
         <v>635252</v>
       </c>
       <c r="D83" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>334</v>
@@ -4755,7 +4755,7 @@
         <v>585442</v>
       </c>
       <c r="D84" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>337</v>
@@ -4790,7 +4790,7 @@
         <v>585546</v>
       </c>
       <c r="D85" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>341</v>
@@ -4825,7 +4825,7 @@
         <v>585404</v>
       </c>
       <c r="D86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>344</v>
@@ -4846,7 +4846,7 @@
         <v>9.56</v>
       </c>
       <c r="K86" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4860,7 +4860,7 @@
         <v>347</v>
       </c>
       <c r="D87" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>348</v>
@@ -4895,7 +4895,7 @@
         <v>545512</v>
       </c>
       <c r="D88" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>352</v>
@@ -4930,7 +4930,7 @@
         <v>545680</v>
       </c>
       <c r="D89" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>356</v>
@@ -4965,7 +4965,7 @@
         <v>359</v>
       </c>
       <c r="D90" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>360</v>
@@ -5000,7 +5000,7 @@
         <v>615362</v>
       </c>
       <c r="D91" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>363</v>
@@ -5021,7 +5021,7 @@
         <v>31.96</v>
       </c>
       <c r="K91" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -5085,7 +5085,7 @@
         <v>4.92</v>
       </c>
       <c r="K93" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -5099,7 +5099,7 @@
         <v>585443</v>
       </c>
       <c r="D94" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>374</v>
@@ -5184,7 +5184,7 @@
         <v>51.6</v>
       </c>
       <c r="K96" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -5198,7 +5198,7 @@
         <v>385</v>
       </c>
       <c r="D97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>386</v>
@@ -5219,7 +5219,7 @@
         <v>9.25</v>
       </c>
       <c r="K97" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -5259,7 +5259,7 @@
         <v>390</v>
       </c>
       <c r="D99" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>391</v>
@@ -5294,7 +5294,7 @@
         <v>585006</v>
       </c>
       <c r="D100" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>394</v>
@@ -5326,7 +5326,7 @@
         <v>396</v>
       </c>
       <c r="D101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>397</v>
@@ -5361,7 +5361,7 @@
         <v>585004</v>
       </c>
       <c r="D102" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>400</v>
@@ -5396,7 +5396,7 @@
         <v>625100</v>
       </c>
       <c r="D103" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>403</v>
@@ -5417,7 +5417,7 @@
         <v>31.96</v>
       </c>
       <c r="K103" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -5545,7 +5545,7 @@
         <v>7.63</v>
       </c>
       <c r="K107" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -5577,7 +5577,7 @@
         <v>29.8</v>
       </c>
       <c r="K108" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -5609,7 +5609,7 @@
         <v>7.76</v>
       </c>
       <c r="K109" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -5623,7 +5623,7 @@
         <v>585444</v>
       </c>
       <c r="D110" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>419</v>
@@ -5658,7 +5658,7 @@
         <v>585450</v>
       </c>
       <c r="D111" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>422</v>
@@ -5693,7 +5693,7 @@
         <v>545532</v>
       </c>
       <c r="D112" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>425</v>
@@ -5728,7 +5728,7 @@
         <v>585592</v>
       </c>
       <c r="D113" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>429</v>
@@ -5763,7 +5763,7 @@
         <v>585468</v>
       </c>
       <c r="D114" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>432</v>
@@ -5795,7 +5795,7 @@
         <v>434</v>
       </c>
       <c r="D115" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>435</v>
@@ -5816,7 +5816,7 @@
         <v>19.96</v>
       </c>
       <c r="K115" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="116" spans="1:11">
@@ -5886,7 +5886,7 @@
         <v>1.4</v>
       </c>
       <c r="K117" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -5929,7 +5929,7 @@
         <v>448</v>
       </c>
       <c r="D119" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>449</v>
@@ -5955,7 +5955,7 @@
         <v>450</v>
       </c>
       <c r="D120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>451</v>
@@ -6022,7 +6022,7 @@
         <v>633126</v>
       </c>
       <c r="D122" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>459</v>
@@ -6057,7 +6057,7 @@
         <v>633134</v>
       </c>
       <c r="D123" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>463</v>
@@ -6078,7 +6078,7 @@
         <v>13.16</v>
       </c>
       <c r="K123" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
     </row>
     <row r="124" spans="1:11">
@@ -6177,7 +6177,7 @@
         <v>1.48</v>
       </c>
       <c r="K126" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="127" spans="1:11">
@@ -6311,7 +6311,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="K130" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -6346,7 +6346,7 @@
         <v>10.82</v>
       </c>
       <c r="K131" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="132" spans="1:11">

</xml_diff>

<commit_message>
Removed duplicated steps for attaching diff pivot.  Fixes #148.
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="521">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -964,6 +964,9 @@
     <t>https://www.servocity.com/770-clamping-hubs#348=107</t>
   </si>
   <si>
+    <t>Differential Pivot, Rocker-Bogie</t>
+  </si>
+  <si>
     <t>4mm Face Tapped Clamp Hub</t>
   </si>
   <si>
@@ -1012,7 +1015,7 @@
     <t>https://www.servocity.com/0-500-1-2-aluminum-tubing#371=455</t>
   </si>
   <si>
-    <t>Body, Differential Pivot</t>
+    <t>Differential Pivot, Mechanical Integration</t>
   </si>
   <si>
     <t>0.5" x 2" aluminum tube</t>
@@ -1066,7 +1069,7 @@
     <t>https://www.servocity.com/aluminum-clamp-collars#368=229</t>
   </si>
   <si>
-    <t>Body, Mechanical Integration, Rocker-Bogie</t>
+    <t>Mechanical Integration, Rocker-Bogie</t>
   </si>
   <si>
     <t>Bore Clamping Hub for 1" PVC</t>
@@ -1522,7 +1525,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Differential Pivot, Corner Steering, Wheel Assembly, Mechanical Integration, Body</t>
+    <t>Differential Pivot, Body, Wheel Assembly, Mechanical Integration, Corner Steering, Rocker-Bogie</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1531,7 +1534,7 @@
     <t>D7</t>
   </si>
   <si>
-    <t>Wheel Assembly, Differential Pivot</t>
+    <t>Differential Pivot, Wheel Assembly</t>
   </si>
   <si>
     <t>Hand Drill or Drill Press</t>
@@ -1552,7 +1555,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Head Assembly, Wheel Assembly, Rocker-Bogie, Differential Pivot</t>
+    <t>Differential Pivot, Wheel Assembly, Rocker-Bogie, Head Assembly</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1567,7 +1570,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Wheel Assembly, Mechanical Integration, Differential Pivot</t>
+    <t>Differential Pivot, Wheel Assembly, Rocker-Bogie, Mechanical Integration</t>
   </si>
   <si>
     <t>Vice or V-Clamp</t>
@@ -1576,7 +1579,7 @@
     <t>D8</t>
   </si>
   <si>
-    <t>Head Assembly, Differential Pivot</t>
+    <t>Differential Pivot, Head Assembly</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2038,7 @@
         <v>100</v>
       </c>
       <c r="G5">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -4519,27 +4522,27 @@
         <v>1</v>
       </c>
       <c r="G77">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H77">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I77" s="1">
         <v>5.99</v>
       </c>
       <c r="J77" s="1">
-        <v>23.96</v>
+        <v>17.97</v>
       </c>
       <c r="K77" t="s">
-        <v>68</v>
+        <v>315</v>
       </c>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B78" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C78">
         <v>545608</v>
@@ -4548,7 +4551,7 @@
         <v>288</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -4571,10 +4574,10 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B79" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C79">
         <v>634070</v>
@@ -4583,7 +4586,7 @@
         <v>288</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -4606,19 +4609,19 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B80" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C80" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -4641,10 +4644,10 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B81" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C81">
         <v>585470</v>
@@ -4653,7 +4656,7 @@
         <v>288</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F81">
         <v>2</v>
@@ -4676,10 +4679,10 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B82" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C82">
         <v>635254</v>
@@ -4688,7 +4691,7 @@
         <v>288</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -4706,15 +4709,15 @@
         <v>10.45</v>
       </c>
       <c r="K82" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B83" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C83">
         <v>635252</v>
@@ -4723,7 +4726,7 @@
         <v>288</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -4746,10 +4749,10 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B84" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C84">
         <v>585442</v>
@@ -4758,7 +4761,7 @@
         <v>288</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -4776,15 +4779,15 @@
         <v>71.81999999999999</v>
       </c>
       <c r="K84" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B85" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C85">
         <v>585546</v>
@@ -4793,33 +4796,33 @@
         <v>288</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="G85">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H85">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I85" s="1">
         <v>5.99</v>
       </c>
       <c r="J85" s="1">
-        <v>23.96</v>
+        <v>11.98</v>
       </c>
       <c r="K85" t="s">
-        <v>331</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B86" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C86">
         <v>585404</v>
@@ -4828,7 +4831,7 @@
         <v>288</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F86">
         <v>2</v>
@@ -4851,19 +4854,19 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B87" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C87" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D87" t="s">
         <v>288</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -4881,15 +4884,15 @@
         <v>27.12</v>
       </c>
       <c r="K87" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B88" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C88">
         <v>545512</v>
@@ -4898,7 +4901,7 @@
         <v>288</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -4916,15 +4919,15 @@
         <v>19.98</v>
       </c>
       <c r="K88" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B89" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C89">
         <v>545680</v>
@@ -4933,7 +4936,7 @@
         <v>288</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -4956,19 +4959,19 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B90" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C90" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D90" t="s">
         <v>288</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -4991,10 +4994,10 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B91" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C91">
         <v>615362</v>
@@ -5003,7 +5006,7 @@
         <v>288</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -5026,16 +5029,16 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B92" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D92" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -5055,19 +5058,19 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B93" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C93" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D93" t="s">
         <v>18</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -5090,10 +5093,10 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B94" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C94">
         <v>585443</v>
@@ -5102,7 +5105,7 @@
         <v>288</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -5125,16 +5128,16 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B95" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D95" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F95">
         <v>2</v>
@@ -5157,16 +5160,16 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B96" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D96" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -5189,19 +5192,19 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B97" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C97" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D97" t="s">
         <v>193</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F97">
         <v>2</v>
@@ -5224,16 +5227,16 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B98" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D98" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -5253,16 +5256,16 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B99" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D99" t="s">
         <v>193</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -5285,10 +5288,10 @@
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B100" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C100">
         <v>585006</v>
@@ -5297,7 +5300,7 @@
         <v>288</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -5320,16 +5323,16 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B101" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D101" t="s">
         <v>193</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -5352,10 +5355,10 @@
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B102" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C102">
         <v>585004</v>
@@ -5364,7 +5367,7 @@
         <v>288</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -5387,10 +5390,10 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B103" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C103">
         <v>625100</v>
@@ -5399,7 +5402,7 @@
         <v>288</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -5422,16 +5425,16 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B104" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D104" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -5454,16 +5457,16 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
+        <v>408</v>
+      </c>
+      <c r="B105" t="s">
+        <v>409</v>
+      </c>
+      <c r="D105" t="s">
+        <v>367</v>
+      </c>
+      <c r="E105" s="5" t="s">
         <v>407</v>
-      </c>
-      <c r="B105" t="s">
-        <v>408</v>
-      </c>
-      <c r="D105" t="s">
-        <v>366</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>406</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -5486,16 +5489,16 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B106" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D106" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -5518,16 +5521,16 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B107" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D107" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -5550,16 +5553,16 @@
     </row>
     <row r="108" spans="1:11">
       <c r="A108" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B108" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D108" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -5582,16 +5585,16 @@
     </row>
     <row r="109" spans="1:11">
       <c r="A109" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B109" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D109" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -5614,10 +5617,10 @@
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B110" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C110">
         <v>585444</v>
@@ -5626,7 +5629,7 @@
         <v>288</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -5649,10 +5652,10 @@
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B111" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C111">
         <v>585450</v>
@@ -5661,7 +5664,7 @@
         <v>288</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -5684,10 +5687,10 @@
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B112" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C112">
         <v>545532</v>
@@ -5696,7 +5699,7 @@
         <v>288</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F112">
         <v>2</v>
@@ -5714,15 +5717,15 @@
         <v>59.85</v>
       </c>
       <c r="K112" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B113" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C113">
         <v>585592</v>
@@ -5731,7 +5734,7 @@
         <v>288</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -5754,10 +5757,10 @@
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B114" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C114">
         <v>585468</v>
@@ -5766,39 +5769,39 @@
         <v>288</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F114">
         <v>1</v>
       </c>
       <c r="G114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I114" s="1">
         <v>1.29</v>
       </c>
       <c r="J114" s="1">
-        <v>2.58</v>
+        <v>1.29</v>
       </c>
       <c r="K114" t="s">
-        <v>331</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B115" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D115" t="s">
         <v>288</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -5821,19 +5824,19 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B116" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C116" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D116" t="s">
         <v>18</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F116">
         <v>100</v>
@@ -5856,19 +5859,19 @@
     </row>
     <row r="117" spans="1:11">
       <c r="A117" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B117" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C117" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D117" t="s">
         <v>18</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F117">
         <v>100</v>
@@ -5891,19 +5894,19 @@
     </row>
     <row r="118" spans="1:11">
       <c r="A118" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B118" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C118" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D118" t="s">
         <v>18</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F118">
         <v>5</v>
@@ -5921,18 +5924,18 @@
         <v>9.880000000000001</v>
       </c>
       <c r="K118" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="119" spans="1:11">
       <c r="A119" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D119" t="s">
         <v>193</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -5952,13 +5955,13 @@
     </row>
     <row r="120" spans="1:11">
       <c r="A120" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D120" t="s">
         <v>193</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -5978,19 +5981,19 @@
     </row>
     <row r="121" spans="1:11">
       <c r="A121" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B121" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C121" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D121" t="s">
         <v>18</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -6008,15 +6011,15 @@
         <v>12.88</v>
       </c>
       <c r="K121" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="122" spans="1:11">
       <c r="A122" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B122" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C122">
         <v>633126</v>
@@ -6025,7 +6028,7 @@
         <v>288</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -6043,15 +6046,15 @@
         <v>3.58</v>
       </c>
       <c r="K122" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="123" spans="1:11">
       <c r="A123" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B123" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C123">
         <v>633134</v>
@@ -6060,7 +6063,7 @@
         <v>288</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F123">
         <v>4</v>
@@ -6083,19 +6086,19 @@
     </row>
     <row r="124" spans="1:11">
       <c r="A124" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B124" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C124" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D124" t="s">
         <v>18</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -6115,19 +6118,19 @@
     </row>
     <row r="125" spans="1:11">
       <c r="A125" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B125" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C125" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D125" t="s">
         <v>18</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -6147,54 +6150,51 @@
     </row>
     <row r="126" spans="1:11">
       <c r="A126" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B126" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C126" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D126" t="s">
         <v>18</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F126">
         <v>1</v>
       </c>
       <c r="G126">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H126">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I126" s="1">
         <v>0.37</v>
       </c>
       <c r="J126" s="1">
-        <v>1.48</v>
-      </c>
-      <c r="K126" t="s">
-        <v>77</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="127" spans="1:11">
       <c r="A127" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B127" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C127" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D127" t="s">
         <v>18</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -6214,51 +6214,54 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B128" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C128" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D128" t="s">
         <v>18</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F128">
         <v>1</v>
       </c>
       <c r="G128">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H128">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I128" s="1">
         <v>0.96</v>
       </c>
       <c r="J128" s="1">
-        <v>0.96</v>
+        <v>3.84</v>
+      </c>
+      <c r="K128" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B129" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C129" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D129" t="s">
         <v>18</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F129">
         <v>1</v>
@@ -6281,19 +6284,19 @@
     </row>
     <row r="130" spans="1:11">
       <c r="A130" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B130" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C130" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D130" t="s">
         <v>18</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F130">
         <v>1</v>
@@ -6316,19 +6319,19 @@
     </row>
     <row r="131" spans="1:11">
       <c r="A131" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B131" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C131" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D131" t="s">
         <v>18</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F131">
         <v>100</v>
@@ -6351,19 +6354,19 @@
     </row>
     <row r="132" spans="1:11">
       <c r="A132" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B132" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C132" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D132" t="s">
         <v>18</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F132">
         <v>100</v>
@@ -6386,114 +6389,114 @@
     </row>
     <row r="133" spans="1:11">
       <c r="A133" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B133" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G133">
         <v>1</v>
       </c>
       <c r="K133" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="134" spans="1:11">
       <c r="A134" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B134" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="G134">
         <v>1</v>
       </c>
       <c r="K134" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="135" spans="1:11">
       <c r="A135" t="s">
+        <v>506</v>
+      </c>
+      <c r="B135" t="s">
+        <v>507</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+      <c r="K135" t="s">
         <v>505</v>
-      </c>
-      <c r="B135" t="s">
-        <v>506</v>
-      </c>
-      <c r="G135">
-        <v>1</v>
-      </c>
-      <c r="K135" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="136" spans="1:11">
       <c r="A136" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B136" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="G136">
         <v>1</v>
       </c>
       <c r="K136" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="137" spans="1:11">
       <c r="A137" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B137" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="G137">
         <v>1</v>
       </c>
       <c r="K137" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="138" spans="1:11">
       <c r="A138" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B138" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G138">
         <v>1</v>
       </c>
       <c r="K138" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="139" spans="1:11">
       <c r="A139" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B139" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="G139">
         <v>1</v>
       </c>
       <c r="K139" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="140" spans="1:11">
       <c r="A140" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B140" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="G140">
         <v>1</v>
       </c>
       <c r="K140" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated prices in master parts list.  Closes #160.
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -1525,7 +1525,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Differential Pivot, Body, Wheel Assembly, Mechanical Integration, Corner Steering, Rocker-Bogie</t>
+    <t>Wheel Assembly, Rocker-Bogie, Differential Pivot, Mechanical Integration, Body, Corner Steering</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1534,7 +1534,7 @@
     <t>D7</t>
   </si>
   <si>
-    <t>Differential Pivot, Wheel Assembly</t>
+    <t>Wheel Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Hand Drill or Drill Press</t>
@@ -1555,7 +1555,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Differential Pivot, Wheel Assembly, Rocker-Bogie, Head Assembly</t>
+    <t>Wheel Assembly, Rocker-Bogie, Differential Pivot, Head Assembly</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1570,7 +1570,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Differential Pivot, Wheel Assembly, Rocker-Bogie, Mechanical Integration</t>
+    <t>Rocker-Bogie, Wheel Assembly, Mechanical Integration, Differential Pivot</t>
   </si>
   <si>
     <t>Vice or V-Clamp</t>
@@ -2289,10 +2289,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>2.87</v>
+        <v>3.02</v>
       </c>
       <c r="J12" s="1">
-        <v>2.87</v>
+        <v>3.02</v>
       </c>
       <c r="K12" t="s">
         <v>55</v>
@@ -4633,10 +4633,10 @@
         <v>1</v>
       </c>
       <c r="I80" s="1">
-        <v>23.16</v>
+        <v>25.74</v>
       </c>
       <c r="J80" s="1">
-        <v>23.16</v>
+        <v>25.74</v>
       </c>
       <c r="K80" t="s">
         <v>50</v>
@@ -4703,10 +4703,10 @@
         <v>5</v>
       </c>
       <c r="I82" s="1">
-        <v>2.09</v>
+        <v>2.19</v>
       </c>
       <c r="J82" s="1">
-        <v>10.45</v>
+        <v>10.95</v>
       </c>
       <c r="K82" t="s">
         <v>332</v>
@@ -4738,10 +4738,10 @@
         <v>1</v>
       </c>
       <c r="I83" s="1">
-        <v>1.49</v>
+        <v>1.59</v>
       </c>
       <c r="J83" s="1">
-        <v>1.49</v>
+        <v>1.59</v>
       </c>
       <c r="K83" t="s">
         <v>301</v>
@@ -4878,10 +4878,10 @@
         <v>12</v>
       </c>
       <c r="I87" s="1">
-        <v>2.26</v>
+        <v>4.99</v>
       </c>
       <c r="J87" s="1">
-        <v>27.12</v>
+        <v>59.88</v>
       </c>
       <c r="K87" t="s">
         <v>350</v>
@@ -4948,10 +4948,10 @@
         <v>6</v>
       </c>
       <c r="I89" s="1">
-        <v>5.99</v>
+        <v>6.99</v>
       </c>
       <c r="J89" s="1">
-        <v>35.94</v>
+        <v>41.94</v>
       </c>
       <c r="K89" t="s">
         <v>30</v>
@@ -4983,10 +4983,10 @@
         <v>4</v>
       </c>
       <c r="I90" s="1">
-        <v>3.69</v>
+        <v>5.2</v>
       </c>
       <c r="J90" s="1">
-        <v>14.76</v>
+        <v>20.8</v>
       </c>
       <c r="K90" t="s">
         <v>30</v>
@@ -5082,10 +5082,10 @@
         <v>1</v>
       </c>
       <c r="I93" s="1">
-        <v>4.92</v>
+        <v>5.28</v>
       </c>
       <c r="J93" s="1">
-        <v>4.92</v>
+        <v>5.28</v>
       </c>
       <c r="K93" t="s">
         <v>82</v>
@@ -5746,10 +5746,10 @@
         <v>8</v>
       </c>
       <c r="I113" s="1">
-        <v>2.79</v>
+        <v>2.89</v>
       </c>
       <c r="J113" s="1">
-        <v>22.32</v>
+        <v>23.12</v>
       </c>
       <c r="K113" t="s">
         <v>35</v>
@@ -5781,10 +5781,10 @@
         <v>1</v>
       </c>
       <c r="I114" s="1">
-        <v>1.29</v>
+        <v>1.49</v>
       </c>
       <c r="J114" s="1">
-        <v>1.29</v>
+        <v>1.49</v>
       </c>
       <c r="K114" t="s">
         <v>50</v>
@@ -5918,10 +5918,10 @@
         <v>4</v>
       </c>
       <c r="I118" s="1">
-        <v>2.47</v>
+        <v>2.59</v>
       </c>
       <c r="J118" s="1">
-        <v>9.880000000000001</v>
+        <v>10.36</v>
       </c>
       <c r="K118" t="s">
         <v>350</v>
@@ -6040,10 +6040,10 @@
         <v>2</v>
       </c>
       <c r="I122" s="1">
-        <v>1.79</v>
+        <v>1.89</v>
       </c>
       <c r="J122" s="1">
-        <v>3.58</v>
+        <v>3.78</v>
       </c>
       <c r="K122" t="s">
         <v>461</v>
@@ -6075,10 +6075,10 @@
         <v>4</v>
       </c>
       <c r="I123" s="1">
-        <v>3.29</v>
+        <v>3.39</v>
       </c>
       <c r="J123" s="1">
-        <v>13.16</v>
+        <v>13.56</v>
       </c>
       <c r="K123" t="s">
         <v>290</v>
@@ -6206,10 +6206,10 @@
         <v>1</v>
       </c>
       <c r="I127" s="1">
-        <v>0.48</v>
+        <v>0.64</v>
       </c>
       <c r="J127" s="1">
-        <v>0.48</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -6238,10 +6238,10 @@
         <v>4</v>
       </c>
       <c r="I128" s="1">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="J128" s="1">
-        <v>3.84</v>
+        <v>4</v>
       </c>
       <c r="K128" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Updated discontinued part.  Closes #184
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="522">
   <si>
     <t>The cost information contained in this document is of a budgetary and planning nature and is intended for informational purposes only.  It does not constitute a commitment on the part of JPL and/or Caltech.</t>
   </si>
@@ -1105,13 +1105,16 @@
     <t>https://www.servocity.com/32-pitch-acetyl-hub-gears-0-1875-face#199=15</t>
   </si>
   <si>
-    <t>Shaft Mount Pinion Gear</t>
+    <t>Shaft Mount Pinion Gear (16 Tooth)</t>
   </si>
   <si>
     <t>S27</t>
   </si>
   <si>
-    <t>https://www.servocity.com/0-125-1-8-bore-32p-shaft-mount-pinion-gear</t>
+    <t>KPL32-32-16</t>
+  </si>
+  <si>
+    <t>https://www.servocity.com/0-125-1-8-bore-32p-shaft-mount-pinion-gears-steel#199=100</t>
   </si>
   <si>
     <t>Custom Acrylic Electronics Board</t>
@@ -1525,7 +1528,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Wheel Assembly, Rocker-Bogie, Differential Pivot, Mechanical Integration, Body, Corner Steering</t>
+    <t>Wheel Assembly, Rocker-Bogie, Corner Steering, Body, Mechanical Integration, Differential Pivot</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1555,7 +1558,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Wheel Assembly, Rocker-Bogie, Differential Pivot, Head Assembly</t>
+    <t>Rocker-Bogie, Head Assembly, Wheel Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1570,7 +1573,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Wheel Assembly, Mechanical Integration, Differential Pivot</t>
+    <t>Rocker-Bogie, Mechanical Integration, Wheel Assembly, Differential Pivot</t>
   </si>
   <si>
     <t>Vice or V-Clamp</t>
@@ -1579,7 +1582,7 @@
     <t>D8</t>
   </si>
   <si>
-    <t>Differential Pivot, Head Assembly</t>
+    <t>Head Assembly, Differential Pivot</t>
   </si>
 </sst>
 </file>
@@ -4999,14 +5002,14 @@
       <c r="B91" t="s">
         <v>363</v>
       </c>
-      <c r="C91">
-        <v>615362</v>
+      <c r="C91" t="s">
+        <v>364</v>
       </c>
       <c r="D91" t="s">
         <v>288</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -5018,10 +5021,10 @@
         <v>4</v>
       </c>
       <c r="I91" s="1">
-        <v>7.99</v>
+        <v>5.99</v>
       </c>
       <c r="J91" s="1">
-        <v>31.96</v>
+        <v>23.96</v>
       </c>
       <c r="K91" t="s">
         <v>290</v>
@@ -5029,16 +5032,16 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B92" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D92" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -5058,19 +5061,19 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B93" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C93" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D93" t="s">
         <v>18</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -5093,10 +5096,10 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B94" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C94">
         <v>585443</v>
@@ -5105,7 +5108,7 @@
         <v>288</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -5128,16 +5131,16 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B95" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D95" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F95">
         <v>2</v>
@@ -5160,16 +5163,16 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B96" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D96" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -5192,19 +5195,19 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B97" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C97" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D97" t="s">
         <v>193</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F97">
         <v>2</v>
@@ -5227,16 +5230,16 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B98" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D98" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -5256,16 +5259,16 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B99" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D99" t="s">
         <v>193</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -5288,10 +5291,10 @@
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B100" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C100">
         <v>585006</v>
@@ -5300,7 +5303,7 @@
         <v>288</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -5323,16 +5326,16 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B101" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D101" t="s">
         <v>193</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -5355,10 +5358,10 @@
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B102" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C102">
         <v>585004</v>
@@ -5367,7 +5370,7 @@
         <v>288</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -5390,10 +5393,10 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B103" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C103">
         <v>625100</v>
@@ -5402,7 +5405,7 @@
         <v>288</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -5425,16 +5428,16 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B104" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D104" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -5457,16 +5460,16 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
+        <v>409</v>
+      </c>
+      <c r="B105" t="s">
+        <v>410</v>
+      </c>
+      <c r="D105" t="s">
+        <v>368</v>
+      </c>
+      <c r="E105" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="B105" t="s">
-        <v>409</v>
-      </c>
-      <c r="D105" t="s">
-        <v>367</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>407</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -5489,16 +5492,16 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B106" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D106" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -5521,16 +5524,16 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B107" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D107" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -5553,16 +5556,16 @@
     </row>
     <row r="108" spans="1:11">
       <c r="A108" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B108" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D108" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -5585,16 +5588,16 @@
     </row>
     <row r="109" spans="1:11">
       <c r="A109" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B109" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D109" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -5617,10 +5620,10 @@
     </row>
     <row r="110" spans="1:11">
       <c r="A110" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B110" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C110">
         <v>585444</v>
@@ -5629,7 +5632,7 @@
         <v>288</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -5652,10 +5655,10 @@
     </row>
     <row r="111" spans="1:11">
       <c r="A111" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B111" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C111">
         <v>585450</v>
@@ -5664,7 +5667,7 @@
         <v>288</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -5687,10 +5690,10 @@
     </row>
     <row r="112" spans="1:11">
       <c r="A112" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B112" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C112">
         <v>545532</v>
@@ -5699,7 +5702,7 @@
         <v>288</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F112">
         <v>2</v>
@@ -5717,15 +5720,15 @@
         <v>59.85</v>
       </c>
       <c r="K112" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B113" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C113">
         <v>585592</v>
@@ -5734,7 +5737,7 @@
         <v>288</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -5757,10 +5760,10 @@
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B114" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C114">
         <v>585468</v>
@@ -5769,7 +5772,7 @@
         <v>288</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -5792,16 +5795,16 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B115" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D115" t="s">
         <v>288</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -5824,19 +5827,19 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B116" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C116" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D116" t="s">
         <v>18</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F116">
         <v>100</v>
@@ -5859,19 +5862,19 @@
     </row>
     <row r="117" spans="1:11">
       <c r="A117" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B117" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C117" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D117" t="s">
         <v>18</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F117">
         <v>100</v>
@@ -5894,19 +5897,19 @@
     </row>
     <row r="118" spans="1:11">
       <c r="A118" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B118" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C118" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D118" t="s">
         <v>18</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F118">
         <v>5</v>
@@ -5929,13 +5932,13 @@
     </row>
     <row r="119" spans="1:11">
       <c r="A119" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D119" t="s">
         <v>193</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -5955,13 +5958,13 @@
     </row>
     <row r="120" spans="1:11">
       <c r="A120" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D120" t="s">
         <v>193</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -5981,19 +5984,19 @@
     </row>
     <row r="121" spans="1:11">
       <c r="A121" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B121" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C121" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D121" t="s">
         <v>18</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -6011,15 +6014,15 @@
         <v>12.88</v>
       </c>
       <c r="K121" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="122" spans="1:11">
       <c r="A122" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B122" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C122">
         <v>633126</v>
@@ -6028,7 +6031,7 @@
         <v>288</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -6046,15 +6049,15 @@
         <v>3.78</v>
       </c>
       <c r="K122" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="123" spans="1:11">
       <c r="A123" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B123" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C123">
         <v>633134</v>
@@ -6063,7 +6066,7 @@
         <v>288</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F123">
         <v>4</v>
@@ -6086,19 +6089,19 @@
     </row>
     <row r="124" spans="1:11">
       <c r="A124" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B124" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C124" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D124" t="s">
         <v>18</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -6118,19 +6121,19 @@
     </row>
     <row r="125" spans="1:11">
       <c r="A125" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B125" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C125" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D125" t="s">
         <v>18</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -6150,19 +6153,19 @@
     </row>
     <row r="126" spans="1:11">
       <c r="A126" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B126" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C126" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D126" t="s">
         <v>18</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -6182,19 +6185,19 @@
     </row>
     <row r="127" spans="1:11">
       <c r="A127" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B127" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C127" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D127" t="s">
         <v>18</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -6214,19 +6217,19 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B128" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C128" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D128" t="s">
         <v>18</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F128">
         <v>1</v>
@@ -6249,19 +6252,19 @@
     </row>
     <row r="129" spans="1:11">
       <c r="A129" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B129" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C129" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D129" t="s">
         <v>18</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F129">
         <v>1</v>
@@ -6284,19 +6287,19 @@
     </row>
     <row r="130" spans="1:11">
       <c r="A130" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B130" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C130" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D130" t="s">
         <v>18</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F130">
         <v>1</v>
@@ -6319,19 +6322,19 @@
     </row>
     <row r="131" spans="1:11">
       <c r="A131" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B131" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C131" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D131" t="s">
         <v>18</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F131">
         <v>100</v>
@@ -6354,19 +6357,19 @@
     </row>
     <row r="132" spans="1:11">
       <c r="A132" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B132" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C132" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D132" t="s">
         <v>18</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F132">
         <v>100</v>
@@ -6389,114 +6392,114 @@
     </row>
     <row r="133" spans="1:11">
       <c r="A133" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B133" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G133">
         <v>1</v>
       </c>
       <c r="K133" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="134" spans="1:11">
       <c r="A134" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B134" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="G134">
         <v>1</v>
       </c>
       <c r="K134" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="135" spans="1:11">
       <c r="A135" t="s">
+        <v>507</v>
+      </c>
+      <c r="B135" t="s">
+        <v>508</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+      <c r="K135" t="s">
         <v>506</v>
-      </c>
-      <c r="B135" t="s">
-        <v>507</v>
-      </c>
-      <c r="G135">
-        <v>1</v>
-      </c>
-      <c r="K135" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="136" spans="1:11">
       <c r="A136" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B136" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G136">
         <v>1</v>
       </c>
       <c r="K136" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="137" spans="1:11">
       <c r="A137" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B137" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="G137">
         <v>1</v>
       </c>
       <c r="K137" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="138" spans="1:11">
       <c r="A138" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B138" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="G138">
         <v>1</v>
       </c>
       <c r="K138" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="139" spans="1:11">
       <c r="A139" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B139" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="G139">
         <v>1</v>
       </c>
       <c r="K139" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="140" spans="1:11">
       <c r="A140" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B140" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="G140">
         <v>1</v>
       </c>
       <c r="K140" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -6588,7 +6591,7 @@
     <hyperlink ref="E88" r:id="rId84"/>
     <hyperlink ref="E89" r:id="rId85"/>
     <hyperlink ref="E90" r:id="rId86" location="199=15"/>
-    <hyperlink ref="E91" r:id="rId87"/>
+    <hyperlink ref="E91" r:id="rId87" location="199=100"/>
     <hyperlink ref="E92" r:id="rId88"/>
     <hyperlink ref="E93" r:id="rId89"/>
     <hyperlink ref="E94" r:id="rId90"/>

</xml_diff>

<commit_message>
Updated PCB parts reference and quantity
</commit_message>
<xml_diff>
--- a/master_parts_list.xlsx
+++ b/master_parts_list.xlsx
@@ -1528,7 +1528,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Wheel Assembly, Rocker-Bogie, Corner Steering, Body, Mechanical Integration, Differential Pivot</t>
+    <t>Wheel Assembly, Corner Steering, Mechanical Integration, Differential Pivot, Rocker-Bogie, Body</t>
   </si>
   <si>
     <t>Center punch or Starter drill bit</t>
@@ -1537,7 +1537,7 @@
     <t>D7</t>
   </si>
   <si>
-    <t>Wheel Assembly, Differential Pivot</t>
+    <t>Differential Pivot, Wheel Assembly</t>
   </si>
   <si>
     <t>Hand Drill or Drill Press</t>
@@ -1558,7 +1558,7 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Head Assembly, Wheel Assembly, Differential Pivot</t>
+    <t>Differential Pivot, Head Assembly, Wheel Assembly, Rocker-Bogie</t>
   </si>
   <si>
     <t>Vice clamp or C Clamps</t>
@@ -1573,7 +1573,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Rocker-Bogie, Mechanical Integration, Wheel Assembly, Differential Pivot</t>
+    <t>Differential Pivot, Wheel Assembly, Rocker-Bogie, Mechanical Integration</t>
   </si>
   <si>
     <t>Vice or V-Clamp</t>
@@ -1582,7 +1582,7 @@
     <t>D8</t>
   </si>
   <si>
-    <t>Head Assembly, Differential Pivot</t>
+    <t>Differential Pivot, Head Assembly</t>
   </si>
 </sst>
 </file>
@@ -6139,16 +6139,19 @@
         <v>1</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I125" s="1">
         <v>0.27</v>
       </c>
       <c r="J125" s="1">
-        <v>0.27</v>
+        <v>5.4</v>
+      </c>
+      <c r="K125" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -6235,19 +6238,16 @@
         <v>1</v>
       </c>
       <c r="G128">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H128">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I128" s="1">
         <v>1</v>
       </c>
       <c r="J128" s="1">
-        <v>4</v>
-      </c>
-      <c r="K128" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -6305,16 +6305,16 @@
         <v>1</v>
       </c>
       <c r="G130">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="H130">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I130" s="1">
         <v>0.41</v>
       </c>
       <c r="J130" s="1">
-        <v>8.199999999999999</v>
+        <v>1.64</v>
       </c>
       <c r="K130" t="s">
         <v>77</v>

</xml_diff>